<commit_message>
Q4 2021 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngcor.xlsx
+++ b/Data/Fiscal Data/ngcor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A308C51-8DA3-44AA-8D95-5723ABC53C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020608CF-D617-41A8-924D-096022F924E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="2025" windowWidth="15540" windowHeight="11385" xr2:uid="{8331D4C4-FE12-4A01-89B6-7737CCA85A42}"/>
+    <workbookView xWindow="5370" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{8331D4C4-FE12-4A01-89B6-7737CCA85A42}"/>
   </bookViews>
   <sheets>
     <sheet name="ngcor" sheetId="1" r:id="rId1"/>
@@ -1892,7 +1892,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="PF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="PO2" sqref="PO2"/>
+      <selection pane="bottomRight" activeCell="PF1" sqref="PF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4492,9 +4492,15 @@
       <c r="PN2" s="2">
         <v>231445</v>
       </c>
-      <c r="PO2" s="2"/>
-      <c r="PP2" s="2"/>
-      <c r="PQ2" s="2"/>
+      <c r="PO2" s="2">
+        <v>253089</v>
+      </c>
+      <c r="PP2" s="2">
+        <v>284014</v>
+      </c>
+      <c r="PQ2" s="2">
+        <v>231310</v>
+      </c>
     </row>
     <row r="3" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5761,35 +5767,41 @@
         <v>209349</v>
       </c>
       <c r="PF3" s="2">
-        <v>231043</v>
+        <v>231038</v>
       </c>
       <c r="PG3" s="2">
-        <v>203282</v>
+        <v>203007</v>
       </c>
       <c r="PH3" s="2">
-        <v>189680</v>
+        <v>189675</v>
       </c>
       <c r="PI3" s="2">
-        <v>271712</v>
+        <v>271706</v>
       </c>
       <c r="PJ3" s="2">
-        <v>234364</v>
+        <v>234357</v>
       </c>
       <c r="PK3" s="2">
-        <v>213677</v>
+        <v>213671</v>
       </c>
       <c r="PL3" s="2">
-        <v>229966</v>
+        <v>230611</v>
       </c>
       <c r="PM3" s="2">
-        <v>240628</v>
+        <v>242356</v>
       </c>
       <c r="PN3" s="2">
-        <v>212681</v>
-      </c>
-      <c r="PO3" s="2"/>
-      <c r="PP3" s="2"/>
-      <c r="PQ3" s="2"/>
+        <v>213506</v>
+      </c>
+      <c r="PO3" s="2">
+        <v>219387</v>
+      </c>
+      <c r="PP3" s="2">
+        <v>269925</v>
+      </c>
+      <c r="PQ3" s="2">
+        <v>223445</v>
+      </c>
     </row>
     <row r="4" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -7082,9 +7094,15 @@
       <c r="PN4" s="2">
         <v>154228</v>
       </c>
-      <c r="PO4" s="2"/>
-      <c r="PP4" s="2"/>
-      <c r="PQ4" s="2"/>
+      <c r="PO4" s="2">
+        <v>162115</v>
+      </c>
+      <c r="PP4" s="2">
+        <v>210746</v>
+      </c>
+      <c r="PQ4" s="2">
+        <v>162331</v>
+      </c>
     </row>
     <row r="5" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -8377,9 +8395,15 @@
       <c r="PN5" s="2">
         <v>57562</v>
       </c>
-      <c r="PO5" s="2"/>
-      <c r="PP5" s="2"/>
-      <c r="PQ5" s="2"/>
+      <c r="PO5" s="2">
+        <v>55532</v>
+      </c>
+      <c r="PP5" s="2">
+        <v>57919</v>
+      </c>
+      <c r="PQ5" s="2">
+        <v>60276</v>
+      </c>
     </row>
     <row r="6" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -9646,35 +9670,41 @@
         <v>652</v>
       </c>
       <c r="PF6" s="2">
-        <v>1623</v>
+        <v>1618</v>
       </c>
       <c r="PG6" s="2">
-        <v>1956</v>
+        <v>1681</v>
       </c>
       <c r="PH6" s="2">
-        <v>1586</v>
+        <v>1581</v>
       </c>
       <c r="PI6" s="2">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="PJ6" s="2">
-        <v>2036</v>
+        <v>2029</v>
       </c>
       <c r="PK6" s="2">
-        <v>2147</v>
+        <v>2141</v>
       </c>
       <c r="PL6" s="2">
-        <v>1964</v>
+        <v>2609</v>
       </c>
       <c r="PM6" s="2">
-        <v>1192</v>
+        <v>2920</v>
       </c>
       <c r="PN6" s="2">
-        <v>891</v>
-      </c>
-      <c r="PO6" s="2"/>
-      <c r="PP6" s="2"/>
-      <c r="PQ6" s="2"/>
+        <v>1716</v>
+      </c>
+      <c r="PO6" s="2">
+        <v>1740</v>
+      </c>
+      <c r="PP6" s="2">
+        <v>1260</v>
+      </c>
+      <c r="PQ6" s="2">
+        <v>838</v>
+      </c>
     </row>
     <row r="7" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -10941,35 +10971,41 @@
         <v>29198</v>
       </c>
       <c r="PF7" s="2">
-        <v>29689</v>
+        <v>29694</v>
       </c>
       <c r="PG7" s="2">
-        <v>16189</v>
+        <v>16464</v>
       </c>
       <c r="PH7" s="2">
-        <v>26472</v>
+        <v>26477</v>
       </c>
       <c r="PI7" s="2">
-        <v>20103</v>
+        <v>20109</v>
       </c>
       <c r="PJ7" s="2">
-        <v>22050.52</v>
+        <v>22057.52</v>
       </c>
       <c r="PK7" s="2">
-        <v>31847</v>
+        <v>31853</v>
       </c>
       <c r="PL7" s="2">
-        <v>26057</v>
+        <v>25412</v>
       </c>
       <c r="PM7" s="2">
-        <v>18621</v>
+        <v>16893</v>
       </c>
       <c r="PN7" s="2">
-        <v>18755</v>
-      </c>
-      <c r="PO7" s="2"/>
-      <c r="PP7" s="2"/>
-      <c r="PQ7" s="2"/>
+        <v>17930</v>
+      </c>
+      <c r="PO7" s="2">
+        <v>33698</v>
+      </c>
+      <c r="PP7" s="2">
+        <v>14075</v>
+      </c>
+      <c r="PQ7" s="2">
+        <v>7838</v>
+      </c>
     </row>
     <row r="8" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -12262,9 +12298,15 @@
       <c r="PN8" s="2">
         <v>9</v>
       </c>
-      <c r="PO8" s="2"/>
-      <c r="PP8" s="2"/>
-      <c r="PQ8" s="2"/>
+      <c r="PO8" s="2">
+        <v>4</v>
+      </c>
+      <c r="PP8" s="2">
+        <v>14</v>
+      </c>
+      <c r="PQ8" s="2">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -13557,9 +13599,15 @@
       <c r="PN9" s="2">
         <v>412361</v>
       </c>
-      <c r="PO9" s="2"/>
-      <c r="PP9" s="2"/>
-      <c r="PQ9" s="2"/>
+      <c r="PO9" s="2">
+        <v>317379</v>
+      </c>
+      <c r="PP9" s="2">
+        <v>412715</v>
+      </c>
+      <c r="PQ9" s="2">
+        <v>569315</v>
+      </c>
     </row>
     <row r="10" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -14852,9 +14900,15 @@
       <c r="PN10" s="2">
         <v>66906</v>
       </c>
-      <c r="PO10" s="2"/>
-      <c r="PP10" s="2"/>
-      <c r="PQ10" s="2"/>
+      <c r="PO10" s="2">
+        <v>65099</v>
+      </c>
+      <c r="PP10" s="2">
+        <v>67208</v>
+      </c>
+      <c r="PQ10" s="2">
+        <v>96656</v>
+      </c>
     </row>
     <row r="11" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -16147,9 +16201,15 @@
       <c r="PN11" s="2">
         <v>47857</v>
       </c>
-      <c r="PO11" s="2"/>
-      <c r="PP11" s="2"/>
-      <c r="PQ11" s="2"/>
+      <c r="PO11" s="2">
+        <v>31536</v>
+      </c>
+      <c r="PP11" s="2">
+        <v>31221</v>
+      </c>
+      <c r="PQ11" s="2">
+        <v>27327</v>
+      </c>
     </row>
     <row r="12" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -17442,9 +17502,15 @@
       <c r="PN12" s="2">
         <v>282111</v>
       </c>
-      <c r="PO12" s="2"/>
-      <c r="PP12" s="2"/>
-      <c r="PQ12" s="2"/>
+      <c r="PO12" s="2">
+        <v>212118</v>
+      </c>
+      <c r="PP12" s="2">
+        <v>296726</v>
+      </c>
+      <c r="PQ12" s="2">
+        <v>418842</v>
+      </c>
     </row>
     <row r="13" spans="1:433" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -18737,9 +18803,15 @@
       <c r="PN13" s="2">
         <v>-180916</v>
       </c>
-      <c r="PO13" s="2"/>
-      <c r="PP13" s="2"/>
-      <c r="PQ13" s="2"/>
+      <c r="PO13" s="2">
+        <v>-64290</v>
+      </c>
+      <c r="PP13" s="2">
+        <v>-128701</v>
+      </c>
+      <c r="PQ13" s="2">
+        <v>-338005</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18749,22 +18821,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A84813-D0CD-4384-80B9-23137239ABCD}">
-  <dimension ref="A1:BD6"/>
+  <dimension ref="A1:BE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BE1" sqref="BE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>420</v>
       </c>
@@ -18933,8 +19005,11 @@
       <c r="BD1">
         <v>2020</v>
       </c>
+      <c r="BE1">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>421</v>
       </c>
@@ -19103,8 +19178,11 @@
       <c r="BD2" s="2">
         <v>2855958.83</v>
       </c>
+      <c r="BE2" s="2">
+        <v>3005538.52</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>422</v>
       </c>
@@ -19271,8 +19349,11 @@
       <c r="BD3" s="2">
         <v>2504421</v>
       </c>
+      <c r="BE3" s="2">
+        <v>2742684</v>
+      </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>426</v>
       </c>
@@ -19439,8 +19520,11 @@
       <c r="BD4" s="2">
         <v>351297</v>
       </c>
+      <c r="BE4" s="2">
+        <v>262500.52</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>445</v>
       </c>
@@ -19609,8 +19693,11 @@
       <c r="BD5" s="2">
         <v>4227406.17</v>
       </c>
+      <c r="BE5" s="2">
+        <v>4675638.54</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>459</v>
       </c>
@@ -19778,6 +19865,9 @@
       </c>
       <c r="BD6" s="2">
         <v>-1371447.3399999999</v>
+      </c>
+      <c r="BE6" s="2">
+        <v>-1670100.02</v>
       </c>
     </row>
   </sheetData>
@@ -19842,7 +19932,7 @@
         <v>464</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Q1 2022 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngcor.xlsx
+++ b/Data/Fiscal Data/ngcor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020608CF-D617-41A8-924D-096022F924E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575D0046-B601-4B43-A0BC-25662A808684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{8331D4C4-FE12-4A01-89B6-7737CCA85A42}"/>
+    <workbookView xWindow="12300" yWindow="1770" windowWidth="8955" windowHeight="11385" xr2:uid="{8331D4C4-FE12-4A01-89B6-7737CCA85A42}"/>
   </bookViews>
   <sheets>
     <sheet name="ngcor" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="499">
   <si>
     <t>January 1986</t>
   </si>
@@ -1490,10 +1490,49 @@
     <t>2015-2021</t>
   </si>
   <si>
-    <t>2000-2021 (Residual calculated for 1986-99)</t>
-  </si>
-  <si>
     <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci0wNTk2NDY1MjcwNTMM</t>
+  </si>
+  <si>
+    <t>January 2022</t>
+  </si>
+  <si>
+    <t>February 2022</t>
+  </si>
+  <si>
+    <t>March 2022</t>
+  </si>
+  <si>
+    <t>April 2022</t>
+  </si>
+  <si>
+    <t>May 2022</t>
+  </si>
+  <si>
+    <t>June 2022</t>
+  </si>
+  <si>
+    <t>July 2022</t>
+  </si>
+  <si>
+    <t>August 2022</t>
+  </si>
+  <si>
+    <t>September 2022</t>
+  </si>
+  <si>
+    <t>October 2022</t>
+  </si>
+  <si>
+    <t>November 2022</t>
+  </si>
+  <si>
+    <t>December 2022</t>
+  </si>
+  <si>
+    <t>1986-2022</t>
+  </si>
+  <si>
+    <t>2000-2022 (Residual calculated for 1986-99)</t>
   </si>
 </sst>
 </file>
@@ -1886,13 +1925,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BD852A-2E1E-45DA-9044-984287FB7C40}">
-  <dimension ref="A1:PQ13"/>
+  <dimension ref="A1:QC13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="PF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="PP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="PF1" sqref="PF1"/>
+      <selection pane="bottomRight" activeCell="PV14" sqref="PV14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,7 +1939,7 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>420</v>
       </c>
@@ -3200,8 +3239,44 @@
       <c r="PQ1" s="1" t="s">
         <v>477</v>
       </c>
+      <c r="PR1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="PS1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="PT1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="PU1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="PV1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="PW1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="PX1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="PY1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="PZ1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="QA1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="QB1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="QC1" s="1" t="s">
+        <v>496</v>
+      </c>
     </row>
-    <row r="2" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>421</v>
       </c>
@@ -4501,8 +4576,28 @@
       <c r="PQ2" s="2">
         <v>231310</v>
       </c>
+      <c r="PR2" s="2">
+        <v>278075</v>
+      </c>
+      <c r="PS2" s="2">
+        <v>212402</v>
+      </c>
+      <c r="PT2" s="2">
+        <v>293883</v>
+      </c>
+      <c r="PU2" s="2">
+        <v>347948.68</v>
+      </c>
+      <c r="PV2" s="2"/>
+      <c r="PW2" s="2"/>
+      <c r="PX2" s="2"/>
+      <c r="PY2" s="2"/>
+      <c r="PZ2" s="2"/>
+      <c r="QA2" s="2"/>
+      <c r="QB2" s="2"/>
+      <c r="QC2" s="2"/>
     </row>
-    <row r="3" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>422</v>
       </c>
@@ -5802,8 +5897,28 @@
       <c r="PQ3" s="2">
         <v>223445</v>
       </c>
+      <c r="PR3" s="2">
+        <v>255294</v>
+      </c>
+      <c r="PS3" s="2">
+        <v>197805</v>
+      </c>
+      <c r="PT3" s="2">
+        <v>244096</v>
+      </c>
+      <c r="PU3" s="2">
+        <v>306896</v>
+      </c>
+      <c r="PV3" s="2"/>
+      <c r="PW3" s="2"/>
+      <c r="PX3" s="2"/>
+      <c r="PY3" s="2"/>
+      <c r="PZ3" s="2"/>
+      <c r="QA3" s="2"/>
+      <c r="QB3" s="2"/>
+      <c r="QC3" s="2"/>
     </row>
-    <row r="4" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>423</v>
       </c>
@@ -7103,8 +7218,28 @@
       <c r="PQ4" s="2">
         <v>162331</v>
       </c>
+      <c r="PR4" s="2">
+        <v>195775</v>
+      </c>
+      <c r="PS4" s="2">
+        <v>136607</v>
+      </c>
+      <c r="PT4" s="2">
+        <v>170384</v>
+      </c>
+      <c r="PU4" s="2">
+        <v>239604</v>
+      </c>
+      <c r="PV4" s="2"/>
+      <c r="PW4" s="2"/>
+      <c r="PX4" s="2"/>
+      <c r="PY4" s="2"/>
+      <c r="PZ4" s="2"/>
+      <c r="QA4" s="2"/>
+      <c r="QB4" s="2"/>
+      <c r="QC4" s="2"/>
     </row>
-    <row r="5" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>424</v>
       </c>
@@ -8404,8 +8539,28 @@
       <c r="PQ5" s="2">
         <v>60276</v>
       </c>
+      <c r="PR5" s="2">
+        <v>58346</v>
+      </c>
+      <c r="PS5" s="2">
+        <v>59433</v>
+      </c>
+      <c r="PT5" s="2">
+        <v>70778</v>
+      </c>
+      <c r="PU5" s="2">
+        <v>65669</v>
+      </c>
+      <c r="PV5" s="2"/>
+      <c r="PW5" s="2"/>
+      <c r="PX5" s="2"/>
+      <c r="PY5" s="2"/>
+      <c r="PZ5" s="2"/>
+      <c r="QA5" s="2"/>
+      <c r="QB5" s="2"/>
+      <c r="QC5" s="2"/>
     </row>
-    <row r="6" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>425</v>
       </c>
@@ -9705,8 +9860,28 @@
       <c r="PQ6" s="2">
         <v>838</v>
       </c>
+      <c r="PR6" s="2">
+        <v>1173</v>
+      </c>
+      <c r="PS6" s="2">
+        <v>1765</v>
+      </c>
+      <c r="PT6" s="2">
+        <v>2934</v>
+      </c>
+      <c r="PU6" s="2">
+        <v>1623</v>
+      </c>
+      <c r="PV6" s="2"/>
+      <c r="PW6" s="2"/>
+      <c r="PX6" s="2"/>
+      <c r="PY6" s="2"/>
+      <c r="PZ6" s="2"/>
+      <c r="QA6" s="2"/>
+      <c r="QB6" s="2"/>
+      <c r="QC6" s="2"/>
     </row>
-    <row r="7" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>426</v>
       </c>
@@ -11006,8 +11181,28 @@
       <c r="PQ7" s="2">
         <v>7838</v>
       </c>
+      <c r="PR7" s="2">
+        <v>22779</v>
+      </c>
+      <c r="PS7" s="2">
+        <v>14538</v>
+      </c>
+      <c r="PT7" s="2">
+        <v>49782</v>
+      </c>
+      <c r="PU7" s="2">
+        <v>40937.68</v>
+      </c>
+      <c r="PV7" s="2"/>
+      <c r="PW7" s="2"/>
+      <c r="PX7" s="2"/>
+      <c r="PY7" s="2"/>
+      <c r="PZ7" s="2"/>
+      <c r="QA7" s="2"/>
+      <c r="QB7" s="2"/>
+      <c r="QC7" s="2"/>
     </row>
-    <row r="8" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>455</v>
       </c>
@@ -12307,8 +12502,28 @@
       <c r="PQ8" s="2">
         <v>27</v>
       </c>
+      <c r="PR8" s="2">
+        <v>2</v>
+      </c>
+      <c r="PS8" s="2">
+        <v>59</v>
+      </c>
+      <c r="PT8" s="2">
+        <v>5</v>
+      </c>
+      <c r="PU8" s="2">
+        <v>115</v>
+      </c>
+      <c r="PV8" s="2"/>
+      <c r="PW8" s="2"/>
+      <c r="PX8" s="2"/>
+      <c r="PY8" s="2"/>
+      <c r="PZ8" s="2"/>
+      <c r="QA8" s="2"/>
+      <c r="QB8" s="2"/>
+      <c r="QC8" s="2"/>
     </row>
-    <row r="9" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>445</v>
       </c>
@@ -13608,8 +13823,28 @@
       <c r="PQ9" s="2">
         <v>569315</v>
       </c>
+      <c r="PR9" s="2">
+        <v>301457</v>
+      </c>
+      <c r="PS9" s="2">
+        <v>318202</v>
+      </c>
+      <c r="PT9" s="2">
+        <v>481549</v>
+      </c>
+      <c r="PU9" s="2">
+        <v>343013</v>
+      </c>
+      <c r="PV9" s="2"/>
+      <c r="PW9" s="2"/>
+      <c r="PX9" s="2"/>
+      <c r="PY9" s="2"/>
+      <c r="PZ9" s="2"/>
+      <c r="QA9" s="2"/>
+      <c r="QB9" s="2"/>
+      <c r="QC9" s="2"/>
     </row>
-    <row r="10" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>456</v>
       </c>
@@ -14909,8 +15144,28 @@
       <c r="PQ10" s="2">
         <v>96656</v>
       </c>
+      <c r="PR10" s="2">
+        <v>79922</v>
+      </c>
+      <c r="PS10" s="2">
+        <v>93367</v>
+      </c>
+      <c r="PT10" s="2">
+        <v>94067</v>
+      </c>
+      <c r="PU10" s="2">
+        <v>85507</v>
+      </c>
+      <c r="PV10" s="2"/>
+      <c r="PW10" s="2"/>
+      <c r="PX10" s="2"/>
+      <c r="PY10" s="2"/>
+      <c r="PZ10" s="2"/>
+      <c r="QA10" s="2"/>
+      <c r="QB10" s="2"/>
+      <c r="QC10" s="2"/>
     </row>
-    <row r="11" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>457</v>
       </c>
@@ -16210,8 +16465,28 @@
       <c r="PQ11" s="2">
         <v>27327</v>
       </c>
+      <c r="PR11" s="2">
+        <v>65551</v>
+      </c>
+      <c r="PS11" s="2">
+        <v>28230</v>
+      </c>
+      <c r="PT11" s="2">
+        <v>55548</v>
+      </c>
+      <c r="PU11" s="2">
+        <v>37303</v>
+      </c>
+      <c r="PV11" s="2"/>
+      <c r="PW11" s="2"/>
+      <c r="PX11" s="2"/>
+      <c r="PY11" s="2"/>
+      <c r="PZ11" s="2"/>
+      <c r="QA11" s="2"/>
+      <c r="QB11" s="2"/>
+      <c r="QC11" s="2"/>
     </row>
-    <row r="12" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>458</v>
       </c>
@@ -17511,8 +17786,28 @@
       <c r="PQ12" s="2">
         <v>418842</v>
       </c>
+      <c r="PR12" s="2">
+        <v>149732</v>
+      </c>
+      <c r="PS12" s="2">
+        <v>188921</v>
+      </c>
+      <c r="PT12" s="2">
+        <v>318734</v>
+      </c>
+      <c r="PU12" s="2">
+        <v>207990</v>
+      </c>
+      <c r="PV12" s="2"/>
+      <c r="PW12" s="2"/>
+      <c r="PX12" s="2"/>
+      <c r="PY12" s="2"/>
+      <c r="PZ12" s="2"/>
+      <c r="QA12" s="2"/>
+      <c r="QB12" s="2"/>
+      <c r="QC12" s="2"/>
     </row>
-    <row r="13" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>459</v>
       </c>
@@ -18812,6 +19107,26 @@
       <c r="PQ13" s="2">
         <v>-338005</v>
       </c>
+      <c r="PR13" s="2">
+        <v>-23382</v>
+      </c>
+      <c r="PS13" s="2">
+        <v>-105800</v>
+      </c>
+      <c r="PT13" s="2">
+        <v>-187666</v>
+      </c>
+      <c r="PU13" s="2">
+        <v>4935.679999999993</v>
+      </c>
+      <c r="PV13" s="2"/>
+      <c r="PW13" s="2"/>
+      <c r="PX13" s="2"/>
+      <c r="PY13" s="2"/>
+      <c r="PZ13" s="2"/>
+      <c r="QA13" s="2"/>
+      <c r="QB13" s="2"/>
+      <c r="QC13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18824,10 +19139,10 @@
   <dimension ref="A1:BE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BE1" sqref="BE1"/>
+      <selection pane="bottomRight" activeCell="BF1" sqref="BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19880,8 +20195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04444F59-DD6B-4831-8845-93AC6460CDAC}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19916,7 +20231,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -19932,7 +20247,7 @@
         <v>464</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -19948,7 +20263,7 @@
         <v>421</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -19956,7 +20271,7 @@
         <v>429</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -19964,7 +20279,7 @@
         <v>430</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -19988,7 +20303,7 @@
         <v>433</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -20004,7 +20319,7 @@
         <v>434</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -20012,7 +20327,7 @@
         <v>435</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -20068,7 +20383,7 @@
         <v>440</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -20076,7 +20391,7 @@
         <v>445</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -20084,7 +20399,7 @@
         <v>446</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -20092,7 +20407,7 @@
         <v>447</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -20132,7 +20447,7 @@
         <v>452</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q4 2023 Fiscal Data Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngcor.xlsx
+++ b/Data/Fiscal Data/ngcor.xlsx
@@ -1,1409 +1,1429 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2D0F57-5F96-47C0-BB7B-0ECFC5EA3427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="615" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ngcor" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Annual" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="metadata" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ngcor" sheetId="1" r:id="rId1"/>
+    <sheet name="Annual" sheetId="2" r:id="rId2"/>
+    <sheet name="metadata" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="511">
   <si>
     <t>Particulars</t>
   </si>
   <si>
-    <t xml:space="preserve">January 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 2023</t>
+    <t>January 1986</t>
+  </si>
+  <si>
+    <t>February 1986</t>
+  </si>
+  <si>
+    <t>March 1986</t>
+  </si>
+  <si>
+    <t>April 1986</t>
+  </si>
+  <si>
+    <t>May 1986</t>
+  </si>
+  <si>
+    <t>June 1986</t>
+  </si>
+  <si>
+    <t>July 1986</t>
+  </si>
+  <si>
+    <t>August 1986</t>
+  </si>
+  <si>
+    <t>September 1986</t>
+  </si>
+  <si>
+    <t>October 1986</t>
+  </si>
+  <si>
+    <t>November 1986</t>
+  </si>
+  <si>
+    <t>December 1986</t>
+  </si>
+  <si>
+    <t>January 1987</t>
+  </si>
+  <si>
+    <t>February 1987</t>
+  </si>
+  <si>
+    <t>March 1987</t>
+  </si>
+  <si>
+    <t>April 1987</t>
+  </si>
+  <si>
+    <t>May 1987</t>
+  </si>
+  <si>
+    <t>June 1987</t>
+  </si>
+  <si>
+    <t>July 1987</t>
+  </si>
+  <si>
+    <t>August 1987</t>
+  </si>
+  <si>
+    <t>September 1987</t>
+  </si>
+  <si>
+    <t>October 1987</t>
+  </si>
+  <si>
+    <t>November 1987</t>
+  </si>
+  <si>
+    <t>December 1987</t>
+  </si>
+  <si>
+    <t>January 1988</t>
+  </si>
+  <si>
+    <t>February 1988</t>
+  </si>
+  <si>
+    <t>March 1988</t>
+  </si>
+  <si>
+    <t>April 1988</t>
+  </si>
+  <si>
+    <t>May 1988</t>
+  </si>
+  <si>
+    <t>June 1988</t>
+  </si>
+  <si>
+    <t>July 1988</t>
+  </si>
+  <si>
+    <t>August 1988</t>
+  </si>
+  <si>
+    <t>September 1988</t>
+  </si>
+  <si>
+    <t>October 1988</t>
+  </si>
+  <si>
+    <t>November 1988</t>
+  </si>
+  <si>
+    <t>December 1988</t>
+  </si>
+  <si>
+    <t>January 1989</t>
+  </si>
+  <si>
+    <t>February 1989</t>
+  </si>
+  <si>
+    <t>March 1989</t>
+  </si>
+  <si>
+    <t>April 1989</t>
+  </si>
+  <si>
+    <t>May 1989</t>
+  </si>
+  <si>
+    <t>June 1989</t>
+  </si>
+  <si>
+    <t>July 1989</t>
+  </si>
+  <si>
+    <t>August 1989</t>
+  </si>
+  <si>
+    <t>September 1989</t>
+  </si>
+  <si>
+    <t>October 1989</t>
+  </si>
+  <si>
+    <t>November 1989</t>
+  </si>
+  <si>
+    <t>December 1989</t>
+  </si>
+  <si>
+    <t>January 1990</t>
+  </si>
+  <si>
+    <t>February 1990</t>
+  </si>
+  <si>
+    <t>March 1990</t>
+  </si>
+  <si>
+    <t>April 1990</t>
+  </si>
+  <si>
+    <t>May 1990</t>
+  </si>
+  <si>
+    <t>June 1990</t>
+  </si>
+  <si>
+    <t>July 1990</t>
+  </si>
+  <si>
+    <t>August 1990</t>
+  </si>
+  <si>
+    <t>September 1990</t>
+  </si>
+  <si>
+    <t>October 1990</t>
+  </si>
+  <si>
+    <t>November 1990</t>
+  </si>
+  <si>
+    <t>December 1990</t>
+  </si>
+  <si>
+    <t>January 1991</t>
+  </si>
+  <si>
+    <t>February 1991</t>
+  </si>
+  <si>
+    <t>March 1991</t>
+  </si>
+  <si>
+    <t>April 1991</t>
+  </si>
+  <si>
+    <t>May 1991</t>
+  </si>
+  <si>
+    <t>June 1991</t>
+  </si>
+  <si>
+    <t>July 1991</t>
+  </si>
+  <si>
+    <t>August 1991</t>
+  </si>
+  <si>
+    <t>September 1991</t>
+  </si>
+  <si>
+    <t>October 1991</t>
+  </si>
+  <si>
+    <t>November 1991</t>
+  </si>
+  <si>
+    <t>December 1991</t>
+  </si>
+  <si>
+    <t>January 1992</t>
+  </si>
+  <si>
+    <t>February 1992</t>
+  </si>
+  <si>
+    <t>March 1992</t>
+  </si>
+  <si>
+    <t>April 1992</t>
+  </si>
+  <si>
+    <t>May 1992</t>
+  </si>
+  <si>
+    <t>June 1992</t>
+  </si>
+  <si>
+    <t>July 1992</t>
+  </si>
+  <si>
+    <t>August 1992</t>
+  </si>
+  <si>
+    <t>September 1992</t>
+  </si>
+  <si>
+    <t>October 1992</t>
+  </si>
+  <si>
+    <t>November 1992</t>
+  </si>
+  <si>
+    <t>December 1992</t>
+  </si>
+  <si>
+    <t>January 1993</t>
+  </si>
+  <si>
+    <t>February 1993</t>
+  </si>
+  <si>
+    <t>March 1993</t>
+  </si>
+  <si>
+    <t>April 1993</t>
+  </si>
+  <si>
+    <t>May 1993</t>
+  </si>
+  <si>
+    <t>June 1993</t>
+  </si>
+  <si>
+    <t>July 1993</t>
+  </si>
+  <si>
+    <t>August 1993</t>
+  </si>
+  <si>
+    <t>September 1993</t>
+  </si>
+  <si>
+    <t>October 1993</t>
+  </si>
+  <si>
+    <t>November 1993</t>
+  </si>
+  <si>
+    <t>December 1993</t>
+  </si>
+  <si>
+    <t>January 1994</t>
+  </si>
+  <si>
+    <t>February 1994</t>
+  </si>
+  <si>
+    <t>March 1994</t>
+  </si>
+  <si>
+    <t>April 1994</t>
+  </si>
+  <si>
+    <t>May 1994</t>
+  </si>
+  <si>
+    <t>June 1994</t>
+  </si>
+  <si>
+    <t>July 1994</t>
+  </si>
+  <si>
+    <t>August 1994</t>
+  </si>
+  <si>
+    <t>September 1994</t>
+  </si>
+  <si>
+    <t>October 1994</t>
+  </si>
+  <si>
+    <t>November 1994</t>
+  </si>
+  <si>
+    <t>December 1994</t>
+  </si>
+  <si>
+    <t>January 1995</t>
+  </si>
+  <si>
+    <t>February 1995</t>
+  </si>
+  <si>
+    <t>March 1995</t>
+  </si>
+  <si>
+    <t>April 1995</t>
+  </si>
+  <si>
+    <t>May 1995</t>
+  </si>
+  <si>
+    <t>June 1995</t>
+  </si>
+  <si>
+    <t>July 1995</t>
+  </si>
+  <si>
+    <t>August 1995</t>
+  </si>
+  <si>
+    <t>September 1995</t>
+  </si>
+  <si>
+    <t>October 1995</t>
+  </si>
+  <si>
+    <t>November 1995</t>
+  </si>
+  <si>
+    <t>December 1995</t>
+  </si>
+  <si>
+    <t>January 1996</t>
+  </si>
+  <si>
+    <t>February 1996</t>
+  </si>
+  <si>
+    <t>March 1996</t>
+  </si>
+  <si>
+    <t>April 1996</t>
+  </si>
+  <si>
+    <t>May 1996</t>
+  </si>
+  <si>
+    <t>June 1996</t>
+  </si>
+  <si>
+    <t>July 1996</t>
+  </si>
+  <si>
+    <t>August 1996</t>
+  </si>
+  <si>
+    <t>September 1996</t>
+  </si>
+  <si>
+    <t>October 1996</t>
+  </si>
+  <si>
+    <t>November 1996</t>
+  </si>
+  <si>
+    <t>December 1996</t>
+  </si>
+  <si>
+    <t>January 1997</t>
+  </si>
+  <si>
+    <t>February 1997</t>
+  </si>
+  <si>
+    <t>March 1997</t>
+  </si>
+  <si>
+    <t>April 1997</t>
+  </si>
+  <si>
+    <t>May 1997</t>
+  </si>
+  <si>
+    <t>June 1997</t>
+  </si>
+  <si>
+    <t>July 1997</t>
+  </si>
+  <si>
+    <t>August 1997</t>
+  </si>
+  <si>
+    <t>September 1997</t>
+  </si>
+  <si>
+    <t>October 1997</t>
+  </si>
+  <si>
+    <t>November 1997</t>
+  </si>
+  <si>
+    <t>December 1997</t>
+  </si>
+  <si>
+    <t>January 1998</t>
+  </si>
+  <si>
+    <t>February 1998</t>
+  </si>
+  <si>
+    <t>March 1998</t>
+  </si>
+  <si>
+    <t>April 1998</t>
+  </si>
+  <si>
+    <t>May 1998</t>
+  </si>
+  <si>
+    <t>June 1998</t>
+  </si>
+  <si>
+    <t>July 1998</t>
+  </si>
+  <si>
+    <t>August 1998</t>
+  </si>
+  <si>
+    <t>September 1998</t>
+  </si>
+  <si>
+    <t>October 1998</t>
+  </si>
+  <si>
+    <t>November 1998</t>
+  </si>
+  <si>
+    <t>December 1998</t>
+  </si>
+  <si>
+    <t>January 1999</t>
+  </si>
+  <si>
+    <t>February 1999</t>
+  </si>
+  <si>
+    <t>March 1999</t>
+  </si>
+  <si>
+    <t>April 1999</t>
+  </si>
+  <si>
+    <t>May 1999</t>
+  </si>
+  <si>
+    <t>June 1999</t>
+  </si>
+  <si>
+    <t>July 1999</t>
+  </si>
+  <si>
+    <t>August 1999</t>
+  </si>
+  <si>
+    <t>September 1999</t>
+  </si>
+  <si>
+    <t>October 1999</t>
+  </si>
+  <si>
+    <t>November 1999</t>
+  </si>
+  <si>
+    <t>December 1999</t>
+  </si>
+  <si>
+    <t>January 2000</t>
+  </si>
+  <si>
+    <t>February 2000</t>
+  </si>
+  <si>
+    <t>March 2000</t>
+  </si>
+  <si>
+    <t>April 2000</t>
+  </si>
+  <si>
+    <t>May 2000</t>
+  </si>
+  <si>
+    <t>June 2000</t>
+  </si>
+  <si>
+    <t>July 2000</t>
+  </si>
+  <si>
+    <t>August 2000</t>
+  </si>
+  <si>
+    <t>September 2000</t>
+  </si>
+  <si>
+    <t>October 2000</t>
+  </si>
+  <si>
+    <t>November 2000</t>
+  </si>
+  <si>
+    <t>December 2000</t>
+  </si>
+  <si>
+    <t>January 2001</t>
+  </si>
+  <si>
+    <t>February 2001</t>
+  </si>
+  <si>
+    <t>March 2001</t>
+  </si>
+  <si>
+    <t>April 2001</t>
+  </si>
+  <si>
+    <t>May 2001</t>
+  </si>
+  <si>
+    <t>June 2001</t>
+  </si>
+  <si>
+    <t>July 2001</t>
+  </si>
+  <si>
+    <t>August 2001</t>
+  </si>
+  <si>
+    <t>September 2001</t>
+  </si>
+  <si>
+    <t>October 2001</t>
+  </si>
+  <si>
+    <t>November 2001</t>
+  </si>
+  <si>
+    <t>December 2001</t>
+  </si>
+  <si>
+    <t>January 2002</t>
+  </si>
+  <si>
+    <t>February 2002</t>
+  </si>
+  <si>
+    <t>March 2002</t>
+  </si>
+  <si>
+    <t>April 2002</t>
+  </si>
+  <si>
+    <t>May 2002</t>
+  </si>
+  <si>
+    <t>June 2002</t>
+  </si>
+  <si>
+    <t>July 2002</t>
+  </si>
+  <si>
+    <t>August 2002</t>
+  </si>
+  <si>
+    <t>September 2002</t>
+  </si>
+  <si>
+    <t>October 2002</t>
+  </si>
+  <si>
+    <t>November 2002</t>
+  </si>
+  <si>
+    <t>December 2002</t>
+  </si>
+  <si>
+    <t>January 2003</t>
+  </si>
+  <si>
+    <t>February 2003</t>
+  </si>
+  <si>
+    <t>March 2003</t>
+  </si>
+  <si>
+    <t>April 2003</t>
+  </si>
+  <si>
+    <t>May 2003</t>
+  </si>
+  <si>
+    <t>June 2003</t>
+  </si>
+  <si>
+    <t>July 2003</t>
+  </si>
+  <si>
+    <t>August 2003</t>
+  </si>
+  <si>
+    <t>September 2003</t>
+  </si>
+  <si>
+    <t>October 2003</t>
+  </si>
+  <si>
+    <t>November 2003</t>
+  </si>
+  <si>
+    <t>December 2003</t>
+  </si>
+  <si>
+    <t>January 2004</t>
+  </si>
+  <si>
+    <t>February 2004</t>
+  </si>
+  <si>
+    <t>March 2004</t>
+  </si>
+  <si>
+    <t>April 2004</t>
+  </si>
+  <si>
+    <t>May 2004</t>
+  </si>
+  <si>
+    <t>June 2004</t>
+  </si>
+  <si>
+    <t>July 2004</t>
+  </si>
+  <si>
+    <t>August 2004</t>
+  </si>
+  <si>
+    <t>September 2004</t>
+  </si>
+  <si>
+    <t>October 2004</t>
+  </si>
+  <si>
+    <t>November 2004</t>
+  </si>
+  <si>
+    <t>December 2004</t>
+  </si>
+  <si>
+    <t>January 2005</t>
+  </si>
+  <si>
+    <t>February 2005</t>
+  </si>
+  <si>
+    <t>March 2005</t>
+  </si>
+  <si>
+    <t>April 2005</t>
+  </si>
+  <si>
+    <t>May 2005</t>
+  </si>
+  <si>
+    <t>June 2005</t>
+  </si>
+  <si>
+    <t>July 2005</t>
+  </si>
+  <si>
+    <t>August 2005</t>
+  </si>
+  <si>
+    <t>September 2005</t>
+  </si>
+  <si>
+    <t>October 2005</t>
+  </si>
+  <si>
+    <t>November 2005</t>
+  </si>
+  <si>
+    <t>December 2005</t>
+  </si>
+  <si>
+    <t>January 2006</t>
+  </si>
+  <si>
+    <t>February 2006</t>
+  </si>
+  <si>
+    <t>March 2006</t>
+  </si>
+  <si>
+    <t>April 2006</t>
+  </si>
+  <si>
+    <t>May 2006</t>
+  </si>
+  <si>
+    <t>June 2006</t>
+  </si>
+  <si>
+    <t>July 2006</t>
+  </si>
+  <si>
+    <t>August 2006</t>
+  </si>
+  <si>
+    <t>September 2006</t>
+  </si>
+  <si>
+    <t>October 2006</t>
+  </si>
+  <si>
+    <t>November 2006</t>
+  </si>
+  <si>
+    <t>December 2006</t>
+  </si>
+  <si>
+    <t>January 2007</t>
+  </si>
+  <si>
+    <t>February 2007</t>
+  </si>
+  <si>
+    <t>March 2007</t>
+  </si>
+  <si>
+    <t>April 2007</t>
+  </si>
+  <si>
+    <t>May 2007</t>
+  </si>
+  <si>
+    <t>June 2007</t>
+  </si>
+  <si>
+    <t>July 2007</t>
+  </si>
+  <si>
+    <t>August 2007</t>
+  </si>
+  <si>
+    <t>September 2007</t>
+  </si>
+  <si>
+    <t>October 2007</t>
+  </si>
+  <si>
+    <t>November 2007</t>
+  </si>
+  <si>
+    <t>December 2007</t>
+  </si>
+  <si>
+    <t>January 2008</t>
+  </si>
+  <si>
+    <t>February 2008</t>
+  </si>
+  <si>
+    <t>March 2008</t>
+  </si>
+  <si>
+    <t>April 2008</t>
+  </si>
+  <si>
+    <t>May 2008</t>
+  </si>
+  <si>
+    <t>June 2008</t>
+  </si>
+  <si>
+    <t>July 2008</t>
+  </si>
+  <si>
+    <t>August 2008</t>
+  </si>
+  <si>
+    <t>September 2008</t>
+  </si>
+  <si>
+    <t>October 2008</t>
+  </si>
+  <si>
+    <t>November 2008</t>
+  </si>
+  <si>
+    <t>December 2008</t>
+  </si>
+  <si>
+    <t>January 2009</t>
+  </si>
+  <si>
+    <t>February 2009</t>
+  </si>
+  <si>
+    <t>March 2009</t>
+  </si>
+  <si>
+    <t>April 2009</t>
+  </si>
+  <si>
+    <t>May 2009</t>
+  </si>
+  <si>
+    <t>June 2009</t>
+  </si>
+  <si>
+    <t>July 2009</t>
+  </si>
+  <si>
+    <t>August 2009</t>
+  </si>
+  <si>
+    <t>September 2009</t>
+  </si>
+  <si>
+    <t>October 2009</t>
+  </si>
+  <si>
+    <t>November 2009</t>
+  </si>
+  <si>
+    <t>December 2009</t>
+  </si>
+  <si>
+    <t>January 2010</t>
+  </si>
+  <si>
+    <t>February 2010</t>
+  </si>
+  <si>
+    <t>March 2010</t>
+  </si>
+  <si>
+    <t>April 2010</t>
+  </si>
+  <si>
+    <t>May 2010</t>
+  </si>
+  <si>
+    <t>June 2010</t>
+  </si>
+  <si>
+    <t>July 2010</t>
+  </si>
+  <si>
+    <t>August 2010</t>
+  </si>
+  <si>
+    <t>September 2010</t>
+  </si>
+  <si>
+    <t>October 2010</t>
+  </si>
+  <si>
+    <t>November 2010</t>
+  </si>
+  <si>
+    <t>December 2010</t>
+  </si>
+  <si>
+    <t>January 2011</t>
+  </si>
+  <si>
+    <t>February 2011</t>
+  </si>
+  <si>
+    <t>March 2011</t>
+  </si>
+  <si>
+    <t>April 2011</t>
+  </si>
+  <si>
+    <t>May 2011</t>
+  </si>
+  <si>
+    <t>June 2011</t>
+  </si>
+  <si>
+    <t>July 2011</t>
+  </si>
+  <si>
+    <t>August 2011</t>
+  </si>
+  <si>
+    <t>September 2011</t>
+  </si>
+  <si>
+    <t>October 2011</t>
+  </si>
+  <si>
+    <t>November 2011</t>
+  </si>
+  <si>
+    <t>December 2011</t>
+  </si>
+  <si>
+    <t>January 2012</t>
+  </si>
+  <si>
+    <t>February 2012</t>
+  </si>
+  <si>
+    <t>March 2012</t>
+  </si>
+  <si>
+    <t>April 2012</t>
+  </si>
+  <si>
+    <t>May 2012</t>
+  </si>
+  <si>
+    <t>June 2012</t>
+  </si>
+  <si>
+    <t>July 2012</t>
+  </si>
+  <si>
+    <t>August 2012</t>
+  </si>
+  <si>
+    <t>September 2012</t>
+  </si>
+  <si>
+    <t>October 2012</t>
+  </si>
+  <si>
+    <t>November 2012</t>
+  </si>
+  <si>
+    <t>December 2012</t>
+  </si>
+  <si>
+    <t>January 2013</t>
+  </si>
+  <si>
+    <t>February 2013</t>
+  </si>
+  <si>
+    <t>March 2013</t>
+  </si>
+  <si>
+    <t>April 2013</t>
+  </si>
+  <si>
+    <t>May 2013</t>
+  </si>
+  <si>
+    <t>June 2013</t>
+  </si>
+  <si>
+    <t>July 2013</t>
+  </si>
+  <si>
+    <t>August 2013</t>
+  </si>
+  <si>
+    <t>September 2013</t>
+  </si>
+  <si>
+    <t>October 2013</t>
+  </si>
+  <si>
+    <t>November 2013</t>
+  </si>
+  <si>
+    <t>December 2013</t>
+  </si>
+  <si>
+    <t>January 2014</t>
+  </si>
+  <si>
+    <t>February 2014</t>
+  </si>
+  <si>
+    <t>March 2014</t>
+  </si>
+  <si>
+    <t>April 2014</t>
+  </si>
+  <si>
+    <t>May 2014</t>
+  </si>
+  <si>
+    <t>June 2014</t>
+  </si>
+  <si>
+    <t>July 2014</t>
+  </si>
+  <si>
+    <t>August 2014</t>
+  </si>
+  <si>
+    <t>September 2014</t>
+  </si>
+  <si>
+    <t>October 2014</t>
+  </si>
+  <si>
+    <t>November 2014</t>
+  </si>
+  <si>
+    <t>December 2014</t>
+  </si>
+  <si>
+    <t>January 2015</t>
+  </si>
+  <si>
+    <t>February 2015</t>
+  </si>
+  <si>
+    <t>March 2015</t>
+  </si>
+  <si>
+    <t>April 2015</t>
+  </si>
+  <si>
+    <t>May 2015</t>
+  </si>
+  <si>
+    <t>June 2015</t>
+  </si>
+  <si>
+    <t>July 2015</t>
+  </si>
+  <si>
+    <t>August 2015</t>
+  </si>
+  <si>
+    <t>September 2015</t>
+  </si>
+  <si>
+    <t>October 2015</t>
+  </si>
+  <si>
+    <t>November 2015</t>
+  </si>
+  <si>
+    <t>December 2015</t>
+  </si>
+  <si>
+    <t>January 2016</t>
+  </si>
+  <si>
+    <t>February 2016</t>
+  </si>
+  <si>
+    <t>March 2016</t>
+  </si>
+  <si>
+    <t>April 2016</t>
+  </si>
+  <si>
+    <t>May 2016</t>
+  </si>
+  <si>
+    <t>June 2016</t>
+  </si>
+  <si>
+    <t>July 2016</t>
+  </si>
+  <si>
+    <t>August 2016</t>
+  </si>
+  <si>
+    <t>September 2016</t>
+  </si>
+  <si>
+    <t>October 2016</t>
+  </si>
+  <si>
+    <t>November 2016</t>
+  </si>
+  <si>
+    <t>December 2016</t>
+  </si>
+  <si>
+    <t>January 2017</t>
+  </si>
+  <si>
+    <t>February 2017</t>
+  </si>
+  <si>
+    <t>March 2017</t>
+  </si>
+  <si>
+    <t>April 2017</t>
+  </si>
+  <si>
+    <t>May 2017</t>
+  </si>
+  <si>
+    <t>June 2017</t>
+  </si>
+  <si>
+    <t>July 2017</t>
+  </si>
+  <si>
+    <t>August 2017</t>
+  </si>
+  <si>
+    <t>September 2017</t>
+  </si>
+  <si>
+    <t>October 2017</t>
+  </si>
+  <si>
+    <t>November 2017</t>
+  </si>
+  <si>
+    <t>December 2017</t>
+  </si>
+  <si>
+    <t>January 2018</t>
+  </si>
+  <si>
+    <t>February 2018</t>
+  </si>
+  <si>
+    <t>March 2018</t>
+  </si>
+  <si>
+    <t>April 2018</t>
+  </si>
+  <si>
+    <t>May 2018</t>
+  </si>
+  <si>
+    <t>June 2018</t>
+  </si>
+  <si>
+    <t>July 2018</t>
+  </si>
+  <si>
+    <t>August 2018</t>
+  </si>
+  <si>
+    <t>September 2018</t>
+  </si>
+  <si>
+    <t>October 2018</t>
+  </si>
+  <si>
+    <t>November 2018</t>
+  </si>
+  <si>
+    <t>December 2018</t>
+  </si>
+  <si>
+    <t>January 2019</t>
+  </si>
+  <si>
+    <t>February 2019</t>
+  </si>
+  <si>
+    <t>March 2019</t>
+  </si>
+  <si>
+    <t>April 2019</t>
+  </si>
+  <si>
+    <t>May 2019</t>
+  </si>
+  <si>
+    <t>June 2019</t>
+  </si>
+  <si>
+    <t>July 2019</t>
+  </si>
+  <si>
+    <t>August 2019</t>
+  </si>
+  <si>
+    <t>September 2019</t>
+  </si>
+  <si>
+    <t>October 2019</t>
+  </si>
+  <si>
+    <t>November 2019</t>
+  </si>
+  <si>
+    <t>December 2019</t>
+  </si>
+  <si>
+    <t>January 2020</t>
+  </si>
+  <si>
+    <t>February 2020</t>
+  </si>
+  <si>
+    <t>March 2020</t>
+  </si>
+  <si>
+    <t>April 2020</t>
+  </si>
+  <si>
+    <t>May 2020</t>
+  </si>
+  <si>
+    <t>June 2020</t>
+  </si>
+  <si>
+    <t>July 2020</t>
+  </si>
+  <si>
+    <t>August 2020</t>
+  </si>
+  <si>
+    <t>September 2020</t>
+  </si>
+  <si>
+    <t>October 2020</t>
+  </si>
+  <si>
+    <t>November 2020</t>
+  </si>
+  <si>
+    <t>December 2020</t>
+  </si>
+  <si>
+    <t>January 2021</t>
+  </si>
+  <si>
+    <t>February 2021</t>
+  </si>
+  <si>
+    <t>March 2021</t>
+  </si>
+  <si>
+    <t>April 2021</t>
+  </si>
+  <si>
+    <t>May 2021</t>
+  </si>
+  <si>
+    <t>June 2021</t>
+  </si>
+  <si>
+    <t>July 2021</t>
+  </si>
+  <si>
+    <t>August 2021</t>
+  </si>
+  <si>
+    <t>September 2021</t>
+  </si>
+  <si>
+    <t>October 2021</t>
+  </si>
+  <si>
+    <t>November 2021</t>
+  </si>
+  <si>
+    <t>December 2021</t>
+  </si>
+  <si>
+    <t>January 2022</t>
+  </si>
+  <si>
+    <t>February 2022</t>
+  </si>
+  <si>
+    <t>March 2022</t>
+  </si>
+  <si>
+    <t>April 2022</t>
+  </si>
+  <si>
+    <t>May 2022</t>
+  </si>
+  <si>
+    <t>June 2022</t>
+  </si>
+  <si>
+    <t>July 2022</t>
+  </si>
+  <si>
+    <t>August 2022</t>
+  </si>
+  <si>
+    <t>September 2022</t>
+  </si>
+  <si>
+    <t>October 2022</t>
+  </si>
+  <si>
+    <t>November 2022</t>
+  </si>
+  <si>
+    <t>December 2022</t>
+  </si>
+  <si>
+    <t>January 2023</t>
+  </si>
+  <si>
+    <t>February 2023</t>
+  </si>
+  <si>
+    <t>March 2023</t>
+  </si>
+  <si>
+    <t>April 2023</t>
+  </si>
+  <si>
+    <t>May 2023</t>
+  </si>
+  <si>
+    <t>June 2023</t>
+  </si>
+  <si>
+    <t>July 2023</t>
+  </si>
+  <si>
+    <t>August 2023</t>
+  </si>
+  <si>
+    <t>September 2023</t>
+  </si>
+  <si>
+    <t>October 2023</t>
+  </si>
+  <si>
+    <t>November 2023</t>
+  </si>
+  <si>
+    <t>December 2023</t>
   </si>
   <si>
     <t>Revenues</t>
   </si>
   <si>
-    <t xml:space="preserve">Tax Revenues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIR Revenues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOC Revenues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Offices Revenues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-tax Revenues</t>
+    <t>Tax Revenues</t>
+  </si>
+  <si>
+    <t>BIR Revenues</t>
+  </si>
+  <si>
+    <t>BOC Revenues</t>
+  </si>
+  <si>
+    <t>Other Offices Revenues</t>
+  </si>
+  <si>
+    <t>Non-tax Revenues</t>
   </si>
   <si>
     <t>Grants</t>
@@ -1412,28 +1432,28 @@
     <t>Expenditures</t>
   </si>
   <si>
-    <t xml:space="preserve">Allotment to LGUs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest Payments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG Disbursements / Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surplus / (Deficit)</t>
+    <t>Allotment to LGUs</t>
+  </si>
+  <si>
+    <t>Interest Payments</t>
+  </si>
+  <si>
+    <t>NG Disbursements / Others</t>
+  </si>
+  <si>
+    <t>Surplus / (Deficit)</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">National Government Cash Operations</t>
+    <t>National Government Cash Operations</t>
   </si>
   <si>
     <t>Source</t>
   </si>
   <si>
-    <t xml:space="preserve">Bureau of Treasury</t>
+    <t>Bureau of Treasury</t>
   </si>
   <si>
     <t>URL</t>
@@ -1448,18 +1468,15 @@
     <t>Units</t>
   </si>
   <si>
-    <t xml:space="preserve">Million Pesos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latest Data</t>
+    <t>Million Pesos</t>
+  </si>
+  <si>
+    <t>Latest Data</t>
   </si>
   <si>
     <t>Availability</t>
   </si>
   <si>
-    <t>1986-2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Tax Revenues</t>
   </si>
   <si>
@@ -1547,34 +1564,37 @@
     <t xml:space="preserve">    NG Disbursements / Others</t>
   </si>
   <si>
-    <t xml:space="preserve">2000-2022 (Residual calculated for 1986-99)</t>
+    <t>1986-2023</t>
+  </si>
+  <si>
+    <t>2000-2023 (Residual calculated for 1986-99)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -1582,7 +1602,13 @@
     <font>
       <b/>
       <u/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -1604,35 +1630,34 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 11" xfId="2"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1640,295 +1665,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2131,23 +1876,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:QO13"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="QF14" activeCellId="0" sqref="QF14"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="PX2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="QF14" sqref="QF14"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.28515625"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3520,7 +3270,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -4716,7 +4466,7 @@
         <v>256742</v>
       </c>
       <c r="OI2" s="2">
-        <v>202085.35000000001</v>
+        <v>202085.35</v>
       </c>
       <c r="OJ2" s="2">
         <v>228918</v>
@@ -4773,7 +4523,7 @@
         <v>243232</v>
       </c>
       <c r="PB2" s="2">
-        <v>212414.82999999999</v>
+        <v>212414.83</v>
       </c>
       <c r="PC2" s="2">
         <v>228206</v>
@@ -4797,7 +4547,7 @@
         <v>291920</v>
       </c>
       <c r="PJ2" s="2">
-        <v>256414.51999999999</v>
+        <v>256414.52</v>
       </c>
       <c r="PK2" s="2">
         <v>245568</v>
@@ -4830,7 +4580,7 @@
         <v>293883</v>
       </c>
       <c r="PU2" s="2">
-        <v>347948.67999999999</v>
+        <v>347948.68</v>
       </c>
       <c r="PV2" s="2">
         <v>304915</v>
@@ -4857,7 +4607,7 @@
         <v>268193</v>
       </c>
       <c r="QD2" s="2">
-        <v>348167</v>
+        <v>348167.25</v>
       </c>
       <c r="QE2" s="2">
         <v>211868</v>
@@ -4866,7 +4616,7 @@
         <v>258650</v>
       </c>
       <c r="QG2" s="2">
-        <v>440697</v>
+        <v>440696.81</v>
       </c>
       <c r="QH2" s="2">
         <v>333437</v>
@@ -4886,10 +4636,14 @@
       <c r="QM2" s="2">
         <v>385808</v>
       </c>
-      <c r="QN2" s="2"/>
-      <c r="QO2" s="2"/>
+      <c r="QN2" s="2">
+        <v>340395</v>
+      </c>
+      <c r="QO2" s="2">
+        <v>260078</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>458</v>
       </c>
@@ -6226,39 +5980,43 @@
         <v>253889</v>
       </c>
       <c r="QD3" s="2">
-        <v>308125</v>
+        <v>308042</v>
       </c>
       <c r="QE3" s="2">
-        <v>194636</v>
+        <v>194642</v>
       </c>
       <c r="QF3" s="2">
-        <v>224380</v>
+        <v>224386</v>
       </c>
       <c r="QG3" s="2">
-        <v>405371</v>
+        <v>405411</v>
       </c>
       <c r="QH3" s="2">
-        <v>294039</v>
+        <v>294048</v>
       </c>
       <c r="QI3" s="2">
-        <v>241043</v>
+        <v>241172</v>
       </c>
       <c r="QJ3" s="2">
-        <v>348507</v>
+        <v>348881</v>
       </c>
       <c r="QK3" s="2">
-        <v>291720</v>
+        <v>291726</v>
       </c>
       <c r="QL3" s="2">
-        <v>233499</v>
+        <v>233532</v>
       </c>
       <c r="QM3" s="2">
-        <v>354737</v>
-      </c>
-      <c r="QN3" s="2"/>
-      <c r="QO3" s="2"/>
+        <v>354763</v>
+      </c>
+      <c r="QN3" s="2">
+        <v>286063</v>
+      </c>
+      <c r="QO3" s="2">
+        <v>246626</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>459</v>
       </c>
@@ -7624,10 +7382,14 @@
       <c r="QM4" s="2">
         <v>274429</v>
       </c>
-      <c r="QN4" s="2"/>
-      <c r="QO4" s="2"/>
+      <c r="QN4" s="2">
+        <v>210242</v>
+      </c>
+      <c r="QO4" s="2">
+        <v>174286</v>
+      </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>460</v>
       </c>
@@ -8993,10 +8755,14 @@
       <c r="QM5" s="2">
         <v>77926</v>
       </c>
-      <c r="QN5" s="2"/>
-      <c r="QO5" s="2"/>
+      <c r="QN5" s="2">
+        <v>73687</v>
+      </c>
+      <c r="QO5" s="2">
+        <v>71213</v>
+      </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -10333,39 +10099,43 @@
         <v>1429</v>
       </c>
       <c r="QD6" s="2">
-        <v>2715</v>
+        <v>2632</v>
       </c>
       <c r="QE6" s="2">
-        <v>2363</v>
+        <v>2369</v>
       </c>
       <c r="QF6" s="2">
-        <v>3075</v>
+        <v>3081</v>
       </c>
       <c r="QG6" s="2">
-        <v>1798</v>
+        <v>1838</v>
       </c>
       <c r="QH6" s="2">
-        <v>2840</v>
+        <v>2849</v>
       </c>
       <c r="QI6" s="2">
-        <v>2182</v>
+        <v>2311</v>
       </c>
       <c r="QJ6" s="2">
-        <v>2315</v>
+        <v>2689</v>
       </c>
       <c r="QK6" s="2">
-        <v>3184</v>
+        <v>3190</v>
       </c>
       <c r="QL6" s="2">
-        <v>2431</v>
+        <v>2464</v>
       </c>
       <c r="QM6" s="2">
-        <v>2382</v>
-      </c>
-      <c r="QN6" s="2"/>
-      <c r="QO6" s="2"/>
+        <v>2408</v>
+      </c>
+      <c r="QN6" s="2">
+        <v>2134</v>
+      </c>
+      <c r="QO6" s="2">
+        <v>1127</v>
+      </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>462</v>
       </c>
@@ -11702,39 +11472,43 @@
         <v>14249</v>
       </c>
       <c r="QD7" s="2">
-        <v>40032</v>
+        <v>40115</v>
       </c>
       <c r="QE7" s="2">
-        <v>17232</v>
+        <v>17226</v>
       </c>
       <c r="QF7" s="2">
-        <v>34270</v>
+        <v>34264</v>
       </c>
       <c r="QG7" s="2">
-        <v>35305</v>
+        <v>35264.81</v>
       </c>
       <c r="QH7" s="2">
-        <v>39382</v>
+        <v>39373</v>
       </c>
       <c r="QI7" s="2">
-        <v>26114</v>
+        <v>25985</v>
       </c>
       <c r="QJ7" s="2">
-        <v>63143</v>
+        <v>62769</v>
       </c>
       <c r="QK7" s="2">
-        <v>18799</v>
+        <v>18793</v>
       </c>
       <c r="QL7" s="2">
-        <v>21666</v>
+        <v>21633</v>
       </c>
       <c r="QM7" s="2">
-        <v>31071</v>
-      </c>
-      <c r="QN7" s="2"/>
-      <c r="QO7" s="2"/>
+        <v>31045</v>
+      </c>
+      <c r="QN7" s="2">
+        <v>54331</v>
+      </c>
+      <c r="QO7" s="2">
+        <v>13365</v>
+      </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>463</v>
       </c>
@@ -12987,7 +12761,7 @@
         <v>102</v>
       </c>
       <c r="PB8" s="2">
-        <v>0.82999999999999996</v>
+        <v>0.83</v>
       </c>
       <c r="PC8" s="2">
         <v>4</v>
@@ -13071,7 +12845,7 @@
         <v>55</v>
       </c>
       <c r="QD8" s="2">
-        <v>10</v>
+        <v>10.25</v>
       </c>
       <c r="QE8" s="2">
         <v>0</v>
@@ -13100,10 +12874,14 @@
       <c r="QM8" s="2">
         <v>0</v>
       </c>
-      <c r="QN8" s="2"/>
-      <c r="QO8" s="2"/>
+      <c r="QN8" s="2">
+        <v>1</v>
+      </c>
+      <c r="QO8" s="2">
+        <v>87</v>
+      </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>464</v>
       </c>
@@ -14068,7 +13846,7 @@
         <v>126885.42600000001</v>
       </c>
       <c r="LJ9" s="2">
-        <v>138142.67999999999</v>
+        <v>138142.68</v>
       </c>
       <c r="LK9" s="2">
         <v>145983.82500000001</v>
@@ -14257,7 +14035,7 @@
         <v>252115</v>
       </c>
       <c r="NU9" s="2">
-        <v>330239.82000000001</v>
+        <v>330239.82</v>
       </c>
       <c r="NV9" s="2">
         <v>228707</v>
@@ -14341,7 +14119,7 @@
         <v>333208</v>
       </c>
       <c r="OW9" s="2">
-        <v>461657.16999999998</v>
+        <v>461657.17</v>
       </c>
       <c r="OX9" s="2">
         <v>353629</v>
@@ -14469,10 +14247,14 @@
       <c r="QM9" s="2">
         <v>420210</v>
       </c>
-      <c r="QN9" s="2"/>
-      <c r="QO9" s="2"/>
+      <c r="QN9" s="2">
+        <v>433649</v>
+      </c>
+      <c r="QO9" s="2">
+        <v>661034</v>
+      </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>465</v>
       </c>
@@ -15838,10 +15620,14 @@
       <c r="QM10" s="2">
         <v>75358</v>
       </c>
-      <c r="QN10" s="2"/>
-      <c r="QO10" s="2"/>
+      <c r="QN10" s="2">
+        <v>80236</v>
+      </c>
+      <c r="QO10" s="2">
+        <v>75878</v>
+      </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>466</v>
       </c>
@@ -17079,7 +16865,7 @@
         <v>43115</v>
       </c>
       <c r="OW11" s="2">
-        <v>21880.169999999998</v>
+        <v>21880.17</v>
       </c>
       <c r="OX11" s="2">
         <v>18353</v>
@@ -17207,10 +16993,14 @@
       <c r="QM11" s="2">
         <v>58983</v>
       </c>
-      <c r="QN11" s="2"/>
-      <c r="QO11" s="2"/>
+      <c r="QN11" s="2">
+        <v>48548</v>
+      </c>
+      <c r="QO11" s="2">
+        <v>60678</v>
+      </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>467</v>
       </c>
@@ -18196,16 +17986,16 @@
         <v>90823.553</v>
       </c>
       <c r="LQ12" s="2">
-        <v>91904.149999999994</v>
+        <v>91904.15</v>
       </c>
       <c r="LR12" s="2">
         <v>115317.58</v>
       </c>
       <c r="LS12" s="2">
-        <v>84386.860000000001</v>
+        <v>84386.86</v>
       </c>
       <c r="LT12" s="2">
-        <v>95691.699999999997</v>
+        <v>95691.7</v>
       </c>
       <c r="LU12" s="2">
         <v>86483</v>
@@ -18576,10 +18366,14 @@
       <c r="QM12" s="2">
         <v>272257</v>
       </c>
-      <c r="QN12" s="2"/>
-      <c r="QO12" s="2"/>
+      <c r="QN12" s="2">
+        <v>289124</v>
+      </c>
+      <c r="QO12" s="2">
+        <v>506658</v>
+      </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:457" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>468</v>
       </c>
@@ -19733,7 +19527,7 @@
         <v>-8623</v>
       </c>
       <c r="NU13" s="2">
-        <v>-107147.82000000001</v>
+        <v>-107147.82</v>
       </c>
       <c r="NV13" s="2">
         <v>10191.130000000005</v>
@@ -19817,7 +19611,7 @@
         <v>-71609</v>
       </c>
       <c r="OW13" s="2">
-        <v>-273881.16999999998</v>
+        <v>-273881.17</v>
       </c>
       <c r="OX13" s="2">
         <v>-202136</v>
@@ -19856,7 +19650,7 @@
         <v>-44426</v>
       </c>
       <c r="PJ13" s="2">
-        <v>-200306.48000000001</v>
+        <v>-200306.48</v>
       </c>
       <c r="PK13" s="2">
         <v>-149862</v>
@@ -19916,7 +19710,7 @@
         <v>-378366</v>
       </c>
       <c r="QD13" s="2">
-        <v>45749</v>
+        <v>45749.25</v>
       </c>
       <c r="QE13" s="2">
         <v>-106373</v>
@@ -19925,7 +19719,7 @@
         <v>-210261</v>
       </c>
       <c r="QG13" s="2">
-        <v>66798</v>
+        <v>66797.81</v>
       </c>
       <c r="QH13" s="2">
         <v>-122231</v>
@@ -19945,32 +19739,39 @@
       <c r="QM13" s="2">
         <v>-34402</v>
       </c>
-      <c r="QN13" s="2"/>
-      <c r="QO13" s="2"/>
+      <c r="QN13" s="2">
+        <v>-93254</v>
+      </c>
+      <c r="QO13" s="2">
+        <v>-400956</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:BG6"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="BF6" activeCellId="0" sqref="BF6"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="BF6" sqref="BF6"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="BG9" sqref="BG9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="2" max="55" width="9.28515625"/>
-    <col bestFit="1" customWidth="1" min="56" max="58" width="9.85546875"/>
+    <col min="2" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20145,8 +19946,11 @@
       <c r="BF1">
         <v>2022</v>
       </c>
+      <c r="BG1">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -20307,22 +20111,25 @@
         <v>2473132</v>
       </c>
       <c r="BB2" s="2">
-        <v>2850184.1299999999</v>
+        <v>2850184.13</v>
       </c>
       <c r="BC2" s="2">
-        <v>3137498.3500000001</v>
+        <v>3137498.35</v>
       </c>
       <c r="BD2" s="2">
-        <v>2855958.8300000001</v>
+        <v>2855958.83</v>
       </c>
       <c r="BE2" s="2">
         <v>3005538.52</v>
       </c>
       <c r="BF2" s="2">
-        <v>3545504.6800000002</v>
+        <v>3545504.68</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>3824105.06</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>458</v>
       </c>
@@ -20495,8 +20302,11 @@
       <c r="BF3" s="2">
         <v>3220315</v>
       </c>
+      <c r="BG3" s="2">
+        <v>3429292</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>462</v>
       </c>
@@ -20664,13 +20474,16 @@
         <v>351297</v>
       </c>
       <c r="BE4" s="2">
-        <v>262500.52000000002</v>
+        <v>262500.52</v>
       </c>
       <c r="BF4" s="2">
-        <v>324081.67999999999</v>
+        <v>324081.68</v>
+      </c>
+      <c r="BG4" s="2">
+        <v>394163.81</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>464</v>
       </c>
@@ -20837,7 +20650,7 @@
         <v>3797734</v>
       </c>
       <c r="BD5" s="2">
-        <v>4227406.1699999999</v>
+        <v>4227406.17</v>
       </c>
       <c r="BE5" s="2">
         <v>4675638.54</v>
@@ -20845,8 +20658,11 @@
       <c r="BF5" s="2">
         <v>5159640</v>
       </c>
+      <c r="BG5" s="2">
+        <v>5336191</v>
+      </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>468</v>
       </c>
@@ -21010,7 +20826,7 @@
         <v>-558258.87</v>
       </c>
       <c r="BC6" s="2">
-        <v>-660235.65000000002</v>
+        <v>-660235.65</v>
       </c>
       <c r="BD6" s="2">
         <v>-1371447.3399999999</v>
@@ -21021,28 +20837,30 @@
       <c r="BF6" s="2">
         <v>-1614135.3199999998</v>
       </c>
+      <c r="BG6" s="2">
+        <v>-1512085.94</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="36.5703125"/>
+    <col min="1" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>469</v>
       </c>
@@ -21050,7 +20868,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>471</v>
       </c>
@@ -21058,7 +20876,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>473</v>
       </c>
@@ -21066,13 +20884,13 @@
         <v>474</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>476</v>
       </c>
@@ -21080,221 +20898,219 @@
         <v>477</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>453</v>
+      <c r="B6" s="1" t="s">
+        <v>456</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>480</v>
       </c>
+      <c r="B10" s="7" t="s">
+        <v>509</v>
+      </c>
     </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>480</v>
+      <c r="B11" s="7" t="s">
+        <v>509</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>482</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>480</v>
+      <c r="B12" t="s">
+        <v>483</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>483</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>484</v>
       </c>
+      <c r="B13" t="s">
+        <v>485</v>
+      </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>485</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>486</v>
       </c>
+      <c r="B14" s="7" t="s">
+        <v>509</v>
+      </c>
     </row>
-    <row r="14">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>484</v>
+      </c>
+      <c r="B15" t="s">
         <v>487</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>480</v>
-      </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>485</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>488</v>
       </c>
+      <c r="B16" s="7" t="s">
+        <v>509</v>
+      </c>
     </row>
-    <row r="16">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>480</v>
+      <c r="B17" s="7" t="s">
+        <v>509</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>490</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>480</v>
+      <c r="B18" t="s">
+        <v>491</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>492</v>
+      </c>
+      <c r="B19" t="s">
         <v>491</v>
       </c>
-      <c r="B18" t="s">
-        <v>492</v>
-      </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>493</v>
       </c>
-      <c r="B19" t="s">
-        <v>492</v>
+      <c r="B20" t="s">
+        <v>494</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>495</v>
+      </c>
+      <c r="B21" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>497</v>
+      </c>
+      <c r="B22" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>499</v>
+      </c>
+      <c r="B23" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>504</v>
+      </c>
+      <c r="B28" t="s">
         <v>494</v>
       </c>
-      <c r="B20" t="s">
-        <v>495</v>
-      </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>496</v>
-      </c>
-      <c r="B21" t="s">
-        <v>497</v>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>505</v>
+      </c>
+      <c r="B29" t="s">
+        <v>491</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>498</v>
-      </c>
-      <c r="B22" t="s">
-        <v>499</v>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>506</v>
+      </c>
+      <c r="B30" t="s">
+        <v>491</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>500</v>
-      </c>
-      <c r="B23" t="s">
-        <v>501</v>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>507</v>
+      </c>
+      <c r="B31" t="s">
+        <v>491</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>505</v>
-      </c>
-      <c r="B28" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>506</v>
-      </c>
-      <c r="B29" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>507</v>
-      </c>
-      <c r="B30" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="B31" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>510</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q1 2024 Fiscal Data Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngcor.xlsx
+++ b/Data/Fiscal Data/ngcor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2D0F57-5F96-47C0-BB7B-0ECFC5EA3427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC16E93-FDF5-4C76-B558-17FD1809D937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8505" yWindow="3870" windowWidth="11145" windowHeight="10185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ngcor" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="523">
   <si>
     <t>Particulars</t>
   </si>
@@ -1568,17 +1568,60 @@
   </si>
   <si>
     <t>2000-2023 (Residual calculated for 1986-99)</t>
+  </si>
+  <si>
+    <t>January 2024</t>
+  </si>
+  <si>
+    <t>February 2024</t>
+  </si>
+  <si>
+    <t>March 2024</t>
+  </si>
+  <si>
+    <t>April 2024</t>
+  </si>
+  <si>
+    <t>May 2024</t>
+  </si>
+  <si>
+    <t>June 2024</t>
+  </si>
+  <si>
+    <t>July 2024</t>
+  </si>
+  <si>
+    <t>August 2024</t>
+  </si>
+  <si>
+    <t>September 2024</t>
+  </si>
+  <si>
+    <t>October 2024</t>
+  </si>
+  <si>
+    <t>November 2024</t>
+  </si>
+  <si>
+    <t>December 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1639,19 +1682,20 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1882,14 +1926,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:QO13"/>
+  <dimension ref="A1:RA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="PX2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="QF14" sqref="QF14"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1941,7 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3269,8 +3313,44 @@
       <c r="QO1" s="1" t="s">
         <v>456</v>
       </c>
+      <c r="QP1" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="QQ1" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="QR1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="QS1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="QT1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="QU1" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="QV1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="QW1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="QX1" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="QY1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="QZ1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="RA1" s="1" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="2" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -4642,8 +4722,26 @@
       <c r="QO2" s="2">
         <v>260078</v>
       </c>
+      <c r="QP2" s="2">
+        <v>421801</v>
+      </c>
+      <c r="QQ2" s="2">
+        <v>224016</v>
+      </c>
+      <c r="QR2" s="2">
+        <v>287923</v>
+      </c>
+      <c r="QS2" s="2"/>
+      <c r="QT2" s="2"/>
+      <c r="QU2" s="2"/>
+      <c r="QV2" s="2"/>
+      <c r="QW2" s="2"/>
+      <c r="QX2" s="2"/>
+      <c r="QY2" s="2"/>
+      <c r="QZ2" s="2"/>
+      <c r="RA2" s="2"/>
     </row>
-    <row r="3" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>458</v>
       </c>
@@ -6015,8 +6113,26 @@
       <c r="QO3" s="2">
         <v>246626</v>
       </c>
+      <c r="QP3" s="2">
+        <v>385159</v>
+      </c>
+      <c r="QQ3" s="2">
+        <v>211305</v>
+      </c>
+      <c r="QR3" s="2">
+        <v>223871</v>
+      </c>
+      <c r="QS3" s="2"/>
+      <c r="QT3" s="2"/>
+      <c r="QU3" s="2"/>
+      <c r="QV3" s="2"/>
+      <c r="QW3" s="2"/>
+      <c r="QX3" s="2"/>
+      <c r="QY3" s="2"/>
+      <c r="QZ3" s="2"/>
+      <c r="RA3" s="2"/>
     </row>
-    <row r="4" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>459</v>
       </c>
@@ -7388,8 +7504,26 @@
       <c r="QO4" s="2">
         <v>174286</v>
       </c>
+      <c r="QP4" s="2">
+        <v>308435</v>
+      </c>
+      <c r="QQ4" s="2">
+        <v>137988</v>
+      </c>
+      <c r="QR4" s="2">
+        <v>145346</v>
+      </c>
+      <c r="QS4" s="2"/>
+      <c r="QT4" s="2"/>
+      <c r="QU4" s="2"/>
+      <c r="QV4" s="2"/>
+      <c r="QW4" s="2"/>
+      <c r="QX4" s="2"/>
+      <c r="QY4" s="2"/>
+      <c r="QZ4" s="2"/>
+      <c r="RA4" s="2"/>
     </row>
-    <row r="5" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>460</v>
       </c>
@@ -8761,8 +8895,26 @@
       <c r="QO5" s="2">
         <v>71213</v>
       </c>
+      <c r="QP5" s="2">
+        <v>73397</v>
+      </c>
+      <c r="QQ5" s="2">
+        <v>70560</v>
+      </c>
+      <c r="QR5" s="2">
+        <v>74895</v>
+      </c>
+      <c r="QS5" s="2"/>
+      <c r="QT5" s="2"/>
+      <c r="QU5" s="2"/>
+      <c r="QV5" s="2"/>
+      <c r="QW5" s="2"/>
+      <c r="QX5" s="2"/>
+      <c r="QY5" s="2"/>
+      <c r="QZ5" s="2"/>
+      <c r="RA5" s="2"/>
     </row>
-    <row r="6" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -10134,8 +10286,26 @@
       <c r="QO6" s="2">
         <v>1127</v>
       </c>
+      <c r="QP6" s="2">
+        <v>3327</v>
+      </c>
+      <c r="QQ6" s="2">
+        <v>2757</v>
+      </c>
+      <c r="QR6" s="2">
+        <v>3630</v>
+      </c>
+      <c r="QS6" s="2"/>
+      <c r="QT6" s="2"/>
+      <c r="QU6" s="2"/>
+      <c r="QV6" s="2"/>
+      <c r="QW6" s="2"/>
+      <c r="QX6" s="2"/>
+      <c r="QY6" s="2"/>
+      <c r="QZ6" s="2"/>
+      <c r="RA6" s="2"/>
     </row>
-    <row r="7" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>462</v>
       </c>
@@ -11507,8 +11677,26 @@
       <c r="QO7" s="2">
         <v>13365</v>
       </c>
+      <c r="QP7" s="2">
+        <v>36641</v>
+      </c>
+      <c r="QQ7" s="2">
+        <v>12711</v>
+      </c>
+      <c r="QR7" s="2">
+        <v>64052</v>
+      </c>
+      <c r="QS7" s="2"/>
+      <c r="QT7" s="2"/>
+      <c r="QU7" s="2"/>
+      <c r="QV7" s="2"/>
+      <c r="QW7" s="2"/>
+      <c r="QX7" s="2"/>
+      <c r="QY7" s="2"/>
+      <c r="QZ7" s="2"/>
+      <c r="RA7" s="2"/>
     </row>
-    <row r="8" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>463</v>
       </c>
@@ -12880,8 +13068,26 @@
       <c r="QO8" s="2">
         <v>87</v>
       </c>
+      <c r="QP8" s="2">
+        <v>1</v>
+      </c>
+      <c r="QQ8" s="2">
+        <v>0</v>
+      </c>
+      <c r="QR8" s="2">
+        <v>0</v>
+      </c>
+      <c r="QS8" s="2"/>
+      <c r="QT8" s="2"/>
+      <c r="QU8" s="2"/>
+      <c r="QV8" s="2"/>
+      <c r="QW8" s="2"/>
+      <c r="QX8" s="2"/>
+      <c r="QY8" s="2"/>
+      <c r="QZ8" s="2"/>
+      <c r="RA8" s="2"/>
     </row>
-    <row r="9" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>464</v>
       </c>
@@ -14253,8 +14459,26 @@
       <c r="QO9" s="2">
         <v>661034</v>
       </c>
+      <c r="QP9" s="2">
+        <v>333850</v>
+      </c>
+      <c r="QQ9" s="2">
+        <v>388693</v>
+      </c>
+      <c r="QR9" s="2">
+        <v>483841</v>
+      </c>
+      <c r="QS9" s="2"/>
+      <c r="QT9" s="2"/>
+      <c r="QU9" s="2"/>
+      <c r="QV9" s="2"/>
+      <c r="QW9" s="2"/>
+      <c r="QX9" s="2"/>
+      <c r="QY9" s="2"/>
+      <c r="QZ9" s="2"/>
+      <c r="RA9" s="2"/>
     </row>
-    <row r="10" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>465</v>
       </c>
@@ -15626,8 +15850,26 @@
       <c r="QO10" s="2">
         <v>75878</v>
       </c>
+      <c r="QP10" s="2">
+        <v>78364</v>
+      </c>
+      <c r="QQ10" s="2">
+        <v>101522</v>
+      </c>
+      <c r="QR10" s="2">
+        <v>80025</v>
+      </c>
+      <c r="QS10" s="2"/>
+      <c r="QT10" s="2"/>
+      <c r="QU10" s="2"/>
+      <c r="QV10" s="2"/>
+      <c r="QW10" s="2"/>
+      <c r="QX10" s="2"/>
+      <c r="QY10" s="2"/>
+      <c r="QZ10" s="2"/>
+      <c r="RA10" s="2"/>
     </row>
-    <row r="11" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>466</v>
       </c>
@@ -16999,8 +17241,26 @@
       <c r="QO11" s="2">
         <v>60678</v>
       </c>
+      <c r="QP11" s="2">
+        <v>74221</v>
+      </c>
+      <c r="QQ11" s="2">
+        <v>47827</v>
+      </c>
+      <c r="QR11" s="2">
+        <v>70944</v>
+      </c>
+      <c r="QS11" s="2"/>
+      <c r="QT11" s="2"/>
+      <c r="QU11" s="2"/>
+      <c r="QV11" s="2"/>
+      <c r="QW11" s="2"/>
+      <c r="QX11" s="2"/>
+      <c r="QY11" s="2"/>
+      <c r="QZ11" s="2"/>
+      <c r="RA11" s="2"/>
     </row>
-    <row r="12" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>467</v>
       </c>
@@ -18372,8 +18632,26 @@
       <c r="QO12" s="2">
         <v>506658</v>
       </c>
+      <c r="QP12" s="2">
+        <v>181265</v>
+      </c>
+      <c r="QQ12" s="2">
+        <v>225033</v>
+      </c>
+      <c r="QR12" s="2">
+        <v>321416</v>
+      </c>
+      <c r="QS12" s="2"/>
+      <c r="QT12" s="2"/>
+      <c r="QU12" s="2"/>
+      <c r="QV12" s="2"/>
+      <c r="QW12" s="2"/>
+      <c r="QX12" s="2"/>
+      <c r="QY12" s="2"/>
+      <c r="QZ12" s="2"/>
+      <c r="RA12" s="2"/>
     </row>
-    <row r="13" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:469" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>468</v>
       </c>
@@ -19745,23 +20023,41 @@
       <c r="QO13" s="2">
         <v>-400956</v>
       </c>
+      <c r="QP13" s="2">
+        <v>87951</v>
+      </c>
+      <c r="QQ13" s="2">
+        <v>-164677</v>
+      </c>
+      <c r="QR13" s="2">
+        <v>-195918</v>
+      </c>
+      <c r="QS13" s="2"/>
+      <c r="QT13" s="2"/>
+      <c r="QU13" s="2"/>
+      <c r="QV13" s="2"/>
+      <c r="QW13" s="2"/>
+      <c r="QX13" s="2"/>
+      <c r="QY13" s="2"/>
+      <c r="QZ13" s="2"/>
+      <c r="RA13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BG6"/>
+  <dimension ref="A1:BG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="BF6" sqref="BF6"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="BG9" sqref="BG9"/>
+      <selection pane="bottomRight" activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20663,181 +20959,320 @@
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2">
+        <v>21612</v>
+      </c>
+      <c r="W6" s="2">
+        <v>36905</v>
+      </c>
+      <c r="X6" s="2">
+        <v>45865</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>54714</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>71114</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>74922</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>79571</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>76491</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>79123</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>72658</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>76522</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>77971</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>99792</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>106290</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>140894</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>174834</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>185861</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>226408</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>260901</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>299807</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>310108</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>267800</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>272218</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>278866</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>294244</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>278996</v>
+      </c>
+      <c r="AV6" s="2">
+        <v>312799</v>
+      </c>
+      <c r="AW6" s="2">
+        <v>323434</v>
+      </c>
+      <c r="AX6" s="2">
+        <v>321185</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>309364</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>304454</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>310541</v>
+      </c>
+      <c r="BB6" s="2">
+        <v>349215</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>360874</v>
+      </c>
+      <c r="BD6" s="2">
+        <v>380412</v>
+      </c>
+      <c r="BE6" s="2">
+        <v>429432</v>
+      </c>
+      <c r="BF6" s="2">
+        <v>502858</v>
+      </c>
+      <c r="BG6" s="2">
+        <v>628333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>468</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>-154</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>-108</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>-19</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>-213</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>-944</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G7" s="2">
         <v>292</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H7" s="2">
         <v>-401</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I7" s="2">
         <v>-360</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J7" s="2">
         <v>686</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K7" s="2">
         <v>-1403</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L7" s="2">
         <v>-2347</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M7" s="2">
         <v>-2862</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N7" s="2">
         <v>-1908</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O7" s="2">
         <v>-342</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P7" s="2">
         <v>-3198</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q7" s="2">
         <v>-12145</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R7" s="2">
         <v>-14404</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S7" s="2">
         <v>-6422</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T7" s="2">
         <v>-10065</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U7" s="2">
         <v>-11141</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V7" s="2">
         <v>-31252</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W7" s="2">
         <v>-16693</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X7" s="2">
         <v>-23206</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y7" s="2">
         <v>-19568</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z7" s="2">
         <v>-37194</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA7" s="2">
         <v>-26349</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB7" s="2">
         <v>-15966</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AC7" s="2">
         <v>-21891</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD7" s="2">
         <v>16286</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AE7" s="2">
         <v>11074</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AF7" s="2">
         <v>6256</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AG7" s="2">
         <v>1564</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="AH7" s="2">
         <v>-49981</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AI7" s="2">
         <v>-111658</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="AJ7" s="2">
         <v>-134212</v>
       </c>
-      <c r="AK6" s="2">
+      <c r="AK7" s="2">
         <v>-147023</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="AL7" s="2">
         <v>-210741</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="AM7" s="2">
         <v>-199868</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="AN7" s="2">
         <v>-187057</v>
       </c>
-      <c r="AO6" s="2">
+      <c r="AO7" s="2">
         <v>-146778</v>
       </c>
-      <c r="AP6" s="2">
+      <c r="AP7" s="2">
         <v>-64791</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AQ7" s="2">
         <v>-12441</v>
       </c>
-      <c r="AR6" s="2">
+      <c r="AR7" s="2">
         <v>-68117</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AS7" s="2">
         <v>-298532</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AT7" s="2">
         <v>-314458</v>
       </c>
-      <c r="AU6" s="2">
+      <c r="AU7" s="2">
         <v>-197754</v>
       </c>
-      <c r="AV6" s="2">
+      <c r="AV7" s="2">
         <v>-242826.61200000002</v>
       </c>
-      <c r="AW6" s="2">
+      <c r="AW7" s="2">
         <v>-164062</v>
       </c>
-      <c r="AX6" s="2">
+      <c r="AX7" s="2">
         <v>-73092</v>
       </c>
-      <c r="AY6" s="2">
+      <c r="AY7" s="2">
         <v>-121689</v>
       </c>
-      <c r="AZ6" s="2">
+      <c r="AZ7" s="2">
         <v>-353422.32299999997</v>
       </c>
-      <c r="BA6" s="2">
+      <c r="BA7" s="2">
         <v>-350637.27300000004</v>
       </c>
-      <c r="BB6" s="2">
+      <c r="BB7" s="2">
         <v>-558258.87</v>
       </c>
-      <c r="BC6" s="2">
+      <c r="BC7" s="2">
         <v>-660235.65</v>
       </c>
-      <c r="BD6" s="2">
+      <c r="BD7" s="2">
         <v>-1371447.3399999999</v>
       </c>
-      <c r="BE6" s="2">
+      <c r="BE7" s="2">
         <v>-1670100.02</v>
       </c>
-      <c r="BF6" s="2">
+      <c r="BF7" s="2">
         <v>-1614135.3199999998</v>
       </c>
-      <c r="BG6" s="2">
+      <c r="BG7" s="2">
         <v>-1512085.94</v>
       </c>
     </row>
@@ -20851,8 +21286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Q1 2025 Fiscal Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngcor.xlsx
+++ b/Data/Fiscal Data/ngcor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0DFAC-854B-4115-A2AE-AFFE4799BA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA657426-8FC1-49AA-AA79-674AB345ACDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13845" yWindow="2295" windowWidth="15270" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ngcor" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="535">
   <si>
     <t>Particulars</t>
   </si>
@@ -1604,6 +1604,42 @@
   </si>
   <si>
     <t>2000-2024 (Residual calculated for 1986-99)</t>
+  </si>
+  <si>
+    <t>January 2025</t>
+  </si>
+  <si>
+    <t>February 2025</t>
+  </si>
+  <si>
+    <t>March 2025</t>
+  </si>
+  <si>
+    <t>April 2025</t>
+  </si>
+  <si>
+    <t>May 2025</t>
+  </si>
+  <si>
+    <t>June 2025</t>
+  </si>
+  <si>
+    <t>July 2025</t>
+  </si>
+  <si>
+    <t>August 2025</t>
+  </si>
+  <si>
+    <t>September 2025</t>
+  </si>
+  <si>
+    <t>October 2025</t>
+  </si>
+  <si>
+    <t>November 2025</t>
+  </si>
+  <si>
+    <t>December 2025</t>
   </si>
 </sst>
 </file>
@@ -1926,14 +1962,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:RA13"/>
+  <dimension ref="A1:RM13"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="QM2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="QZ2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="QF14" sqref="QF14"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="QP14" sqref="QP14"/>
+      <selection pane="bottomRight" activeCell="RE10" sqref="RE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1977,7 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3349,8 +3385,44 @@
       <c r="RA1" s="1" t="s">
         <v>520</v>
       </c>
+      <c r="RB1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="RC1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="RD1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="RE1" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="RF1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="RG1" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="RH1" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="RI1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="RJ1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="RK1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="RL1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="RM1" s="1" t="s">
+        <v>534</v>
+      </c>
     </row>
-    <row r="2" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -4758,8 +4830,26 @@
       <c r="RA2" s="2">
         <v>314674</v>
       </c>
+      <c r="RB2" s="2">
+        <v>467146.65</v>
+      </c>
+      <c r="RC2" s="2">
+        <v>251766.92636559001</v>
+      </c>
+      <c r="RD2" s="2">
+        <v>279253</v>
+      </c>
+      <c r="RE2" s="2"/>
+      <c r="RF2" s="2"/>
+      <c r="RG2" s="2"/>
+      <c r="RH2" s="2"/>
+      <c r="RI2" s="2"/>
+      <c r="RJ2" s="2"/>
+      <c r="RK2" s="2"/>
+      <c r="RL2" s="2"/>
+      <c r="RM2" s="2"/>
     </row>
-    <row r="3" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>458</v>
       </c>
@@ -6167,8 +6257,26 @@
       <c r="RA3" s="2">
         <v>251587</v>
       </c>
+      <c r="RB3" s="2">
+        <v>437534.65</v>
+      </c>
+      <c r="RC3" s="2">
+        <v>234346.92636559001</v>
+      </c>
+      <c r="RD3" s="2">
+        <v>259630</v>
+      </c>
+      <c r="RE3" s="2"/>
+      <c r="RF3" s="2"/>
+      <c r="RG3" s="2"/>
+      <c r="RH3" s="2"/>
+      <c r="RI3" s="2"/>
+      <c r="RJ3" s="2"/>
+      <c r="RK3" s="2"/>
+      <c r="RL3" s="2"/>
+      <c r="RM3" s="2"/>
     </row>
-    <row r="4" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>459</v>
       </c>
@@ -7576,8 +7684,26 @@
       <c r="RA4" s="2">
         <v>183839</v>
       </c>
+      <c r="RB4" s="2">
+        <v>355095.65</v>
+      </c>
+      <c r="RC4" s="2">
+        <v>159652.92636559001</v>
+      </c>
+      <c r="RD4" s="2">
+        <v>175660</v>
+      </c>
+      <c r="RE4" s="2"/>
+      <c r="RF4" s="2"/>
+      <c r="RG4" s="2"/>
+      <c r="RH4" s="2"/>
+      <c r="RI4" s="2"/>
+      <c r="RJ4" s="2"/>
+      <c r="RK4" s="2"/>
+      <c r="RL4" s="2"/>
+      <c r="RM4" s="2"/>
     </row>
-    <row r="5" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>460</v>
       </c>
@@ -8985,8 +9111,26 @@
       <c r="RA5" s="2">
         <v>66672</v>
       </c>
+      <c r="RB5" s="2">
+        <v>79254</v>
+      </c>
+      <c r="RC5" s="2">
+        <v>71765</v>
+      </c>
+      <c r="RD5" s="2">
+        <v>80359</v>
+      </c>
+      <c r="RE5" s="2"/>
+      <c r="RF5" s="2"/>
+      <c r="RG5" s="2"/>
+      <c r="RH5" s="2"/>
+      <c r="RI5" s="2"/>
+      <c r="RJ5" s="2"/>
+      <c r="RK5" s="2"/>
+      <c r="RL5" s="2"/>
+      <c r="RM5" s="2"/>
     </row>
-    <row r="6" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>461</v>
       </c>
@@ -10394,8 +10538,26 @@
       <c r="RA6" s="2">
         <v>1076</v>
       </c>
+      <c r="RB6" s="2">
+        <v>3185</v>
+      </c>
+      <c r="RC6" s="2">
+        <v>2929</v>
+      </c>
+      <c r="RD6" s="2">
+        <v>3611</v>
+      </c>
+      <c r="RE6" s="2"/>
+      <c r="RF6" s="2"/>
+      <c r="RG6" s="2"/>
+      <c r="RH6" s="2"/>
+      <c r="RI6" s="2"/>
+      <c r="RJ6" s="2"/>
+      <c r="RK6" s="2"/>
+      <c r="RL6" s="2"/>
+      <c r="RM6" s="2"/>
     </row>
-    <row r="7" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>462</v>
       </c>
@@ -11803,8 +11965,26 @@
       <c r="RA7" s="2">
         <v>63086</v>
       </c>
+      <c r="RB7" s="2">
+        <v>29612</v>
+      </c>
+      <c r="RC7" s="2">
+        <v>17420</v>
+      </c>
+      <c r="RD7" s="2">
+        <v>19623</v>
+      </c>
+      <c r="RE7" s="2"/>
+      <c r="RF7" s="2"/>
+      <c r="RG7" s="2"/>
+      <c r="RH7" s="2"/>
+      <c r="RI7" s="2"/>
+      <c r="RJ7" s="2"/>
+      <c r="RK7" s="2"/>
+      <c r="RL7" s="2"/>
+      <c r="RM7" s="2"/>
     </row>
-    <row r="8" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>463</v>
       </c>
@@ -13212,8 +13392,26 @@
       <c r="RA8" s="2">
         <v>1</v>
       </c>
+      <c r="RB8" s="2">
+        <v>0</v>
+      </c>
+      <c r="RC8" s="2">
+        <v>66</v>
+      </c>
+      <c r="RD8" s="2">
+        <v>1</v>
+      </c>
+      <c r="RE8" s="2"/>
+      <c r="RF8" s="2"/>
+      <c r="RG8" s="2"/>
+      <c r="RH8" s="2"/>
+      <c r="RI8" s="2"/>
+      <c r="RJ8" s="2"/>
+      <c r="RK8" s="2"/>
+      <c r="RL8" s="2"/>
+      <c r="RM8" s="2"/>
     </row>
-    <row r="9" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>464</v>
       </c>
@@ -14621,8 +14819,26 @@
       <c r="RA9" s="2">
         <v>644175</v>
       </c>
+      <c r="RB9" s="2">
+        <v>398785</v>
+      </c>
+      <c r="RC9" s="2">
+        <v>423211</v>
+      </c>
+      <c r="RD9" s="2">
+        <v>654984</v>
+      </c>
+      <c r="RE9" s="2"/>
+      <c r="RF9" s="2"/>
+      <c r="RG9" s="2"/>
+      <c r="RH9" s="2"/>
+      <c r="RI9" s="2"/>
+      <c r="RJ9" s="2"/>
+      <c r="RK9" s="2"/>
+      <c r="RL9" s="2"/>
+      <c r="RM9" s="2"/>
     </row>
-    <row r="10" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>465</v>
       </c>
@@ -16030,8 +16246,26 @@
       <c r="RA10" s="2">
         <v>82811</v>
       </c>
+      <c r="RB10" s="2">
+        <v>86112</v>
+      </c>
+      <c r="RC10" s="2">
+        <v>102016</v>
+      </c>
+      <c r="RD10" s="2">
+        <v>101127</v>
+      </c>
+      <c r="RE10" s="2"/>
+      <c r="RF10" s="2"/>
+      <c r="RG10" s="2"/>
+      <c r="RH10" s="2"/>
+      <c r="RI10" s="2"/>
+      <c r="RJ10" s="2"/>
+      <c r="RK10" s="2"/>
+      <c r="RL10" s="2"/>
+      <c r="RM10" s="2"/>
     </row>
-    <row r="11" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>466</v>
       </c>
@@ -17439,8 +17673,26 @@
       <c r="RA11" s="2">
         <v>57979</v>
       </c>
+      <c r="RB11" s="2">
+        <v>104435</v>
+      </c>
+      <c r="RC11" s="2">
+        <v>48445</v>
+      </c>
+      <c r="RD11" s="2">
+        <v>88121</v>
+      </c>
+      <c r="RE11" s="2"/>
+      <c r="RF11" s="2"/>
+      <c r="RG11" s="2"/>
+      <c r="RH11" s="2"/>
+      <c r="RI11" s="2"/>
+      <c r="RJ11" s="2"/>
+      <c r="RK11" s="2"/>
+      <c r="RL11" s="2"/>
+      <c r="RM11" s="2"/>
     </row>
-    <row r="12" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>467</v>
       </c>
@@ -18848,8 +19100,26 @@
       <c r="RA12" s="2">
         <v>485320</v>
       </c>
+      <c r="RB12" s="2">
+        <v>203853</v>
+      </c>
+      <c r="RC12" s="2">
+        <v>255957</v>
+      </c>
+      <c r="RD12" s="2">
+        <v>451652</v>
+      </c>
+      <c r="RE12" s="2"/>
+      <c r="RF12" s="2"/>
+      <c r="RG12" s="2"/>
+      <c r="RH12" s="2"/>
+      <c r="RI12" s="2"/>
+      <c r="RJ12" s="2"/>
+      <c r="RK12" s="2"/>
+      <c r="RL12" s="2"/>
+      <c r="RM12" s="2"/>
     </row>
-    <row r="13" spans="1:469" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:481" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>468</v>
       </c>
@@ -20257,6 +20527,24 @@
       <c r="RA13" s="2">
         <v>-329501</v>
       </c>
+      <c r="RB13" s="2">
+        <v>68361.650000000023</v>
+      </c>
+      <c r="RC13" s="2">
+        <v>-171444.07363440999</v>
+      </c>
+      <c r="RD13" s="2">
+        <v>-375731</v>
+      </c>
+      <c r="RE13" s="2"/>
+      <c r="RF13" s="2"/>
+      <c r="RG13" s="2"/>
+      <c r="RH13" s="2"/>
+      <c r="RI13" s="2"/>
+      <c r="RJ13" s="2"/>
+      <c r="RK13" s="2"/>
+      <c r="RL13" s="2"/>
+      <c r="RM13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21523,7 +21811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Monthly inflation update - Dec 2025
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngcor.xlsx
+++ b/Data/Fiscal Data/ngcor.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F7D539-69AD-4501-90DC-8AC6D2073342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F529D8C3-A119-4D99-AD2C-19F01B543E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="14715" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="4185" windowWidth="14715" windowHeight="9525" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ngcor" sheetId="1" r:id="rId1"/>
     <sheet name="Annual" sheetId="2" r:id="rId2"/>
-    <sheet name="metadata" sheetId="3" r:id="rId3"/>
+    <sheet name="annual_psy" sheetId="4" r:id="rId3"/>
+    <sheet name="annual_cbp" sheetId="5" r:id="rId4"/>
+    <sheet name="metadata" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="540">
   <si>
     <t>Particulars</t>
   </si>
@@ -1640,13 +1642,28 @@
   </si>
   <si>
     <t>December 2025</t>
+  </si>
+  <si>
+    <t>Primary Balance</t>
+  </si>
+  <si>
+    <t>PSY1990</t>
+  </si>
+  <si>
+    <t>PSY1987</t>
+  </si>
+  <si>
+    <t>PSY1981,1980</t>
+  </si>
+  <si>
+    <t>PSY1971</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1661,21 +1678,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1684,16 +1711,33 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1704,6 +1748,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1718,20 +1768,24 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1964,12 +2018,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:RM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="QZ2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="QF14" sqref="QF14"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="RB1" sqref="RB1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20698,18 +20752,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BH7"/>
+  <dimension ref="A1:BH8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="BF6" sqref="BF6"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="BH8" sqref="BH8"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="55" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="56" max="58" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="59" max="60" width="9.85546875" customWidth="1"/>
@@ -20901,43 +20956,43 @@
       <c r="A2" t="s">
         <v>457</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="9">
         <v>309</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="9">
         <v>795</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="9">
         <v>1265</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="9">
         <v>2093</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="9">
         <v>3611</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="9">
         <v>5265</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="9">
         <v>5873</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="9">
         <v>7695</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="9">
         <v>12157</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="9">
         <v>16856</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="9">
         <v>18090</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="9">
         <v>19959</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="9">
         <v>24103</v>
       </c>
       <c r="O2" s="2">
@@ -20947,13 +21002,13 @@
         <v>34077</v>
       </c>
       <c r="Q2" s="2">
-        <v>34600</v>
+        <v>34599</v>
       </c>
       <c r="R2" s="2">
         <v>38206</v>
       </c>
       <c r="S2" s="2">
-        <v>46641</v>
+        <v>45632</v>
       </c>
       <c r="T2" s="2">
         <v>56861</v>
@@ -21083,41 +21138,41 @@
       <c r="A3" t="s">
         <v>458</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="9">
         <v>269</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="9">
         <v>682</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="9">
         <v>997</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="9">
         <v>1754</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="9">
         <v>3228</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9">
         <v>4998</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="9">
         <v>6438</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="9">
         <v>10370</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="9">
         <v>13753</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="9">
         <v>15368</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="9">
         <v>16955</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="9">
         <v>20445</v>
       </c>
       <c r="O3" s="2">
@@ -21263,41 +21318,41 @@
       <c r="A4" t="s">
         <v>462</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="9">
         <v>40</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="9">
         <v>113</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="9">
         <v>268</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="9">
         <v>339</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="9">
         <v>383</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
         <v>875</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="9">
         <v>1258</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="9">
         <v>1787</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="9">
         <v>3103</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="9">
         <v>2722</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="9">
         <v>3004</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="9">
         <v>3658</v>
       </c>
       <c r="O4" s="2">
@@ -21443,43 +21498,43 @@
       <c r="A5" t="s">
         <v>464</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="9">
         <v>463</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="9">
         <v>903</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="9">
         <v>1284</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="9">
         <v>2306</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="9">
         <v>4555</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="9">
         <v>4973</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="9">
         <v>6274</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="9">
         <v>8055</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="9">
         <v>11471</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="9">
         <v>18259</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="9">
         <v>20437</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="9">
         <v>22821</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="9">
         <v>26011</v>
       </c>
       <c r="O5" s="2">
@@ -21495,7 +21550,7 @@
         <v>52610</v>
       </c>
       <c r="S5" s="2">
-        <v>53063</v>
+        <v>53065</v>
       </c>
       <c r="T5" s="2">
         <v>66926</v>
@@ -21625,26 +21680,40 @@
       <c r="A6" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="2">
+        <v>1841</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2296</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2429</v>
+      </c>
+      <c r="R6" s="2">
+        <v>3560</v>
+      </c>
+      <c r="S6" s="2">
+        <v>4997</v>
+      </c>
+      <c r="T6" s="2">
+        <v>10409</v>
+      </c>
+      <c r="U6" s="2">
+        <v>14652</v>
+      </c>
       <c r="V6" s="2">
         <v>21612</v>
       </c>
@@ -21767,43 +21836,43 @@
       <c r="A7" t="s">
         <v>468</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="9">
         <v>-154</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="9">
         <v>-108</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="9">
         <v>-19</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="9">
         <v>-213</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="9">
         <v>-944</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="9">
         <v>292</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="9">
         <v>-401</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="9">
         <v>-360</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="9">
         <v>686</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="9">
         <v>-1403</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="9">
         <v>-2347</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="9">
         <v>-2862</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="9">
         <v>-1908</v>
       </c>
       <c r="O7" s="2">
@@ -21813,13 +21882,13 @@
         <v>-3198</v>
       </c>
       <c r="Q7" s="2">
-        <v>-12145</v>
+        <v>-12146</v>
       </c>
       <c r="R7" s="2">
         <v>-14404</v>
       </c>
       <c r="S7" s="2">
-        <v>-6422</v>
+        <v>-7433</v>
       </c>
       <c r="T7" s="2">
         <v>-10065</v>
@@ -21943,6 +22012,195 @@
       </c>
       <c r="BH7" s="2">
         <v>-1506358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="O8" s="2">
+        <f>O7+O6</f>
+        <v>1499</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" ref="P8:BH8" si="0">P7+P6</f>
+        <v>-902</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>-9717</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="0"/>
+        <v>-10844</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="0"/>
+        <v>-2436</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="0"/>
+        <v>3511</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="0"/>
+        <v>-9640</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" si="0"/>
+        <v>20212</v>
+      </c>
+      <c r="X8" s="2">
+        <f t="shared" si="0"/>
+        <v>22659</v>
+      </c>
+      <c r="Y8" s="2">
+        <f t="shared" si="0"/>
+        <v>35146</v>
+      </c>
+      <c r="Z8" s="2">
+        <f t="shared" si="0"/>
+        <v>33920</v>
+      </c>
+      <c r="AA8" s="2">
+        <f t="shared" si="0"/>
+        <v>48573</v>
+      </c>
+      <c r="AB8" s="2">
+        <f t="shared" si="0"/>
+        <v>63605</v>
+      </c>
+      <c r="AC8" s="2">
+        <f t="shared" si="0"/>
+        <v>54600</v>
+      </c>
+      <c r="AD8" s="2">
+        <f t="shared" si="0"/>
+        <v>95409</v>
+      </c>
+      <c r="AE8" s="2">
+        <f t="shared" si="0"/>
+        <v>83732</v>
+      </c>
+      <c r="AF8" s="2">
+        <f t="shared" si="0"/>
+        <v>82778</v>
+      </c>
+      <c r="AG8" s="2">
+        <f t="shared" si="0"/>
+        <v>79535</v>
+      </c>
+      <c r="AH8" s="2">
+        <f t="shared" si="0"/>
+        <v>49811</v>
+      </c>
+      <c r="AI8" s="2">
+        <f t="shared" si="0"/>
+        <v>-5368</v>
+      </c>
+      <c r="AJ8" s="2">
+        <f t="shared" si="0"/>
+        <v>6682</v>
+      </c>
+      <c r="AK8" s="2">
+        <f t="shared" si="0"/>
+        <v>27811</v>
+      </c>
+      <c r="AL8" s="2">
+        <f t="shared" si="0"/>
+        <v>-24880</v>
+      </c>
+      <c r="AM8" s="2">
+        <f t="shared" si="0"/>
+        <v>26540</v>
+      </c>
+      <c r="AN8" s="2">
+        <f t="shared" si="0"/>
+        <v>73844</v>
+      </c>
+      <c r="AO8" s="2">
+        <f t="shared" si="0"/>
+        <v>153029</v>
+      </c>
+      <c r="AP8" s="2">
+        <f t="shared" si="0"/>
+        <v>245317</v>
+      </c>
+      <c r="AQ8" s="2">
+        <f t="shared" si="0"/>
+        <v>255359</v>
+      </c>
+      <c r="AR8" s="2">
+        <f t="shared" si="0"/>
+        <v>204101</v>
+      </c>
+      <c r="AS8" s="2">
+        <f t="shared" si="0"/>
+        <v>-19666</v>
+      </c>
+      <c r="AT8" s="2">
+        <f t="shared" si="0"/>
+        <v>-20214</v>
+      </c>
+      <c r="AU8" s="2">
+        <f t="shared" si="0"/>
+        <v>81242</v>
+      </c>
+      <c r="AV8" s="2">
+        <f t="shared" si="0"/>
+        <v>69972.387999999977</v>
+      </c>
+      <c r="AW8" s="2">
+        <f t="shared" si="0"/>
+        <v>159372</v>
+      </c>
+      <c r="AX8" s="2">
+        <f t="shared" si="0"/>
+        <v>248093</v>
+      </c>
+      <c r="AY8" s="2">
+        <f t="shared" si="0"/>
+        <v>187675</v>
+      </c>
+      <c r="AZ8" s="2">
+        <f t="shared" si="0"/>
+        <v>-48968.322999999975</v>
+      </c>
+      <c r="BA8" s="2">
+        <f t="shared" si="0"/>
+        <v>-40096.273000000045</v>
+      </c>
+      <c r="BB8" s="2">
+        <f t="shared" si="0"/>
+        <v>-209043.87</v>
+      </c>
+      <c r="BC8" s="2">
+        <f t="shared" si="0"/>
+        <v>-299361.65000000002</v>
+      </c>
+      <c r="BD8" s="2">
+        <f t="shared" si="0"/>
+        <v>-991035.33999999985</v>
+      </c>
+      <c r="BE8" s="2">
+        <f t="shared" si="0"/>
+        <v>-1240668.02</v>
+      </c>
+      <c r="BF8" s="2">
+        <f t="shared" si="0"/>
+        <v>-1111277.3199999998</v>
+      </c>
+      <c r="BG8" s="2">
+        <f t="shared" si="0"/>
+        <v>-883752.94</v>
+      </c>
+      <c r="BH8" s="2">
+        <f t="shared" si="0"/>
+        <v>-743045</v>
       </c>
     </row>
   </sheetData>
@@ -21952,6 +22210,1195 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3E5222-E6F5-4037-9D06-FF5A6DA63AFD}">
+  <dimension ref="A1:X16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="23" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1965</v>
+      </c>
+      <c r="C1">
+        <v>1966</v>
+      </c>
+      <c r="D1">
+        <v>1967</v>
+      </c>
+      <c r="E1">
+        <v>1968</v>
+      </c>
+      <c r="F1">
+        <v>1969</v>
+      </c>
+      <c r="G1">
+        <v>1970</v>
+      </c>
+      <c r="H1">
+        <v>1971</v>
+      </c>
+      <c r="I1">
+        <v>1972</v>
+      </c>
+      <c r="J1">
+        <v>1973</v>
+      </c>
+      <c r="K1">
+        <v>1974</v>
+      </c>
+      <c r="L1">
+        <v>1975</v>
+      </c>
+      <c r="M1">
+        <v>1976</v>
+      </c>
+      <c r="N1">
+        <v>1977</v>
+      </c>
+      <c r="O1">
+        <v>1978</v>
+      </c>
+      <c r="P1">
+        <v>1979</v>
+      </c>
+      <c r="Q1">
+        <v>1980</v>
+      </c>
+      <c r="R1">
+        <v>1981</v>
+      </c>
+      <c r="S1">
+        <v>1982</v>
+      </c>
+      <c r="T1">
+        <v>1983</v>
+      </c>
+      <c r="U1">
+        <v>1984</v>
+      </c>
+      <c r="V1">
+        <v>1985</v>
+      </c>
+      <c r="W1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>1552.2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1928.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2105.1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2364.6</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <v>16784</v>
+      </c>
+      <c r="M2" s="2">
+        <v>18159</v>
+      </c>
+      <c r="N2" s="2">
+        <v>18605</v>
+      </c>
+      <c r="O2" s="2">
+        <v>24103</v>
+      </c>
+      <c r="P2" s="2">
+        <v>29470</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>34077</v>
+      </c>
+      <c r="R2" s="2">
+        <v>34600</v>
+      </c>
+      <c r="S2" s="2">
+        <v>38306</v>
+      </c>
+      <c r="T2" s="2">
+        <v>46641</v>
+      </c>
+      <c r="U2" s="2">
+        <v>59861</v>
+      </c>
+      <c r="V2" s="2">
+        <v>67958</v>
+      </c>
+      <c r="W2" s="2">
+        <v>79245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1524</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1413.9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1705.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1885.06</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2167.1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>2726</v>
+      </c>
+      <c r="H3" s="11">
+        <v>3825</v>
+      </c>
+      <c r="I3" s="11">
+        <v>4387</v>
+      </c>
+      <c r="J3" s="11">
+        <v>6239</v>
+      </c>
+      <c r="K3" s="11">
+        <v>10094</v>
+      </c>
+      <c r="L3" s="2">
+        <v>13723</v>
+      </c>
+      <c r="M3" s="2">
+        <v>15788</v>
+      </c>
+      <c r="N3" s="2">
+        <v>17024</v>
+      </c>
+      <c r="O3" s="2">
+        <v>20445</v>
+      </c>
+      <c r="P3" s="2">
+        <v>25525</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>28833</v>
+      </c>
+      <c r="R3" s="2">
+        <v>30062</v>
+      </c>
+      <c r="S3" s="2">
+        <v>33900</v>
+      </c>
+      <c r="T3" s="2">
+        <v>39848</v>
+      </c>
+      <c r="U3" s="2">
+        <v>50118</v>
+      </c>
+      <c r="V3" s="2">
+        <v>60253</v>
+      </c>
+      <c r="W3" s="2">
+        <v>65491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
+        <f>120.5+18.3</f>
+        <v>138.80000000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <f>221.8+1.1</f>
+        <v>222.9</v>
+      </c>
+      <c r="E4" s="2">
+        <v>218</v>
+      </c>
+      <c r="F4" s="2">
+        <v>196</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>3061</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2371</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1581</v>
+      </c>
+      <c r="O4" s="2">
+        <v>3658</v>
+      </c>
+      <c r="P4" s="2">
+        <v>3945</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>5244</v>
+      </c>
+      <c r="R4" s="2">
+        <v>4538</v>
+      </c>
+      <c r="S4" s="2">
+        <v>4406</v>
+      </c>
+      <c r="T4" s="2">
+        <v>6793</v>
+      </c>
+      <c r="U4" s="2">
+        <v>6743</v>
+      </c>
+      <c r="V4" s="2">
+        <v>7705</v>
+      </c>
+      <c r="W4" s="2">
+        <v>13754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2077.3000000000002</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1893.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2043.2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2332.1799999999998</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3019.2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4053.5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4429</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5588.2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>8574.2000000000007</v>
+      </c>
+      <c r="K5" s="2">
+        <v>13024.7</v>
+      </c>
+      <c r="L5" s="2">
+        <v>19049</v>
+      </c>
+      <c r="M5" s="2">
+        <v>22418.1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>22596.3</v>
+      </c>
+      <c r="O5" s="2">
+        <v>28066</v>
+      </c>
+      <c r="P5" s="2">
+        <v>34154</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>38079</v>
+      </c>
+      <c r="R5" s="2">
+        <v>49083</v>
+      </c>
+      <c r="S5" s="2">
+        <v>51142</v>
+      </c>
+      <c r="T5" s="2">
+        <v>55811</v>
+      </c>
+      <c r="U5" s="2">
+        <v>68625</v>
+      </c>
+      <c r="V5" s="2">
+        <v>87390</v>
+      </c>
+      <c r="W5" s="2">
+        <v>114505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B6" s="2">
+        <v>56.7</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>148.80000000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>212.8</v>
+      </c>
+      <c r="I6" s="2">
+        <v>327.9</v>
+      </c>
+      <c r="J6" s="2">
+        <v>295.3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>376.6</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
+        <v>745.6</v>
+      </c>
+      <c r="N6" s="2">
+        <v>819.2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1136</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1841</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2296</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2429</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3560</v>
+      </c>
+      <c r="T6" s="2">
+        <v>4997</v>
+      </c>
+      <c r="U6" s="2">
+        <v>10409</v>
+      </c>
+      <c r="V6" s="2">
+        <v>14652</v>
+      </c>
+      <c r="W6" s="2">
+        <v>21612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>468</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:F7" si="0">C2-C5</f>
+        <v>-341.29999999999995</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>-114.70000000000005</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>-227.07999999999993</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>-654.59999999999991</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
+        <f t="shared" ref="L7:N7" si="1">L2-L5</f>
+        <v>-2265</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="1"/>
+        <v>-4259.0999999999985</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="1"/>
+        <v>-3991.2999999999993</v>
+      </c>
+      <c r="O7" s="2">
+        <f>O2-O5</f>
+        <v>-3963</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" ref="P7:W7" si="2">P2-P5</f>
+        <v>-4684</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="2"/>
+        <v>-4002</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="2"/>
+        <v>-14483</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="2"/>
+        <v>-12836</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="2"/>
+        <v>-9170</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="2"/>
+        <v>-8764</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" si="2"/>
+        <v>-19432</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" si="2"/>
+        <v>-35260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <f t="shared" ref="L8:V8" si="3">L7+L6</f>
+        <v>-2265</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="3"/>
+        <v>-3513.4999999999986</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="3"/>
+        <v>-3172.0999999999995</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="3"/>
+        <v>-2827</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="3"/>
+        <v>-2843</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="3"/>
+        <v>-1706</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="3"/>
+        <v>-12054</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
+        <v>-9276</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="3"/>
+        <v>-4173</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="3"/>
+        <v>1645</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="3"/>
+        <v>-4780</v>
+      </c>
+      <c r="W8" s="2">
+        <f>W7+W6</f>
+        <v>-13648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>539</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2ECE54-8573-4B6F-A9C3-5B4E9249FD2A}">
+  <dimension ref="A1:W8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="23" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1965</v>
+      </c>
+      <c r="C1">
+        <v>1966</v>
+      </c>
+      <c r="D1">
+        <v>1967</v>
+      </c>
+      <c r="E1">
+        <v>1968</v>
+      </c>
+      <c r="F1">
+        <v>1969</v>
+      </c>
+      <c r="G1">
+        <v>1970</v>
+      </c>
+      <c r="H1">
+        <v>1971</v>
+      </c>
+      <c r="I1">
+        <v>1972</v>
+      </c>
+      <c r="J1">
+        <v>1973</v>
+      </c>
+      <c r="K1">
+        <v>1974</v>
+      </c>
+      <c r="L1">
+        <v>1975</v>
+      </c>
+      <c r="M1">
+        <v>1976</v>
+      </c>
+      <c r="N1">
+        <v>1977</v>
+      </c>
+      <c r="O1">
+        <v>1978</v>
+      </c>
+      <c r="P1">
+        <v>1979</v>
+      </c>
+      <c r="Q1">
+        <v>1980</v>
+      </c>
+      <c r="R1">
+        <v>1981</v>
+      </c>
+      <c r="S1">
+        <v>1982</v>
+      </c>
+      <c r="T1">
+        <v>1983</v>
+      </c>
+      <c r="U1">
+        <v>1984</v>
+      </c>
+      <c r="V1">
+        <v>1985</v>
+      </c>
+      <c r="W1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1863.7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1867.5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2339.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2553.1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2862.3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3109.9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4296.8</v>
+      </c>
+      <c r="I2" s="12">
+        <f>H2*(I3/H3)</f>
+        <v>4922.5867913195616</v>
+      </c>
+      <c r="J2" s="2">
+        <f>K2-6628</f>
+        <v>11094</v>
+      </c>
+      <c r="K2" s="2">
+        <v>17722</v>
+      </c>
+      <c r="L2" s="2">
+        <f>10691.2+10734.5</f>
+        <v>21425.7</v>
+      </c>
+      <c r="M2" s="2">
+        <v>21027</v>
+      </c>
+      <c r="N2" s="2">
+        <v>24802</v>
+      </c>
+      <c r="O2" s="2">
+        <v>29804.5</v>
+      </c>
+      <c r="P2" s="2">
+        <v>35258.699999999997</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>45816.2</v>
+      </c>
+      <c r="R2" s="2">
+        <v>35933</v>
+      </c>
+      <c r="S2" s="2">
+        <v>38205</v>
+      </c>
+      <c r="T2" s="2">
+        <v>46641</v>
+      </c>
+      <c r="U2" s="2">
+        <v>57927</v>
+      </c>
+      <c r="V2" s="2">
+        <v>68961</v>
+      </c>
+      <c r="W2" s="2">
+        <v>79245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1523.7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1559.7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1915.2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2156.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2475.1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2725.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3829.3</v>
+      </c>
+      <c r="I3" s="12">
+        <f>annual_psy!I3</f>
+        <v>4387</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
+        <v>31423</v>
+      </c>
+      <c r="S3" s="2">
+        <v>33795</v>
+      </c>
+      <c r="T3" s="2">
+        <v>39598</v>
+      </c>
+      <c r="U3" s="2">
+        <v>50751</v>
+      </c>
+      <c r="V3" s="2">
+        <v>61190</v>
+      </c>
+      <c r="W3" s="2">
+        <v>65491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B4" s="2">
+        <v>322.8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>274.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>323</v>
+      </c>
+      <c r="E4" s="2">
+        <v>339.8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>387.2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>384.8</v>
+      </c>
+      <c r="H4" s="2">
+        <v>467.5</v>
+      </c>
+      <c r="I4" s="12">
+        <f>(I3/H3)*H4</f>
+        <v>535.58679131956228</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2">
+        <v>4510</v>
+      </c>
+      <c r="S4" s="2">
+        <v>4410</v>
+      </c>
+      <c r="T4" s="2">
+        <v>7043</v>
+      </c>
+      <c r="U4" s="2">
+        <v>7176</v>
+      </c>
+      <c r="V4" s="2">
+        <v>7771</v>
+      </c>
+      <c r="W4" s="2">
+        <v>13754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2109.6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2244.1999999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2607.6999999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2997.9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3678.3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4107.6000000000004</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4480.6000000000004</v>
+      </c>
+      <c r="I5" s="12">
+        <f>annual_psy!I5</f>
+        <v>5588.2</v>
+      </c>
+      <c r="J5" s="2">
+        <f>K5-6180</f>
+        <v>8974</v>
+      </c>
+      <c r="K5" s="2">
+        <v>15154</v>
+      </c>
+      <c r="L5" s="2">
+        <f>9650.9+12501.2</f>
+        <v>22152.1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>23048.2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>26636</v>
+      </c>
+      <c r="O5" s="2">
+        <v>31363.7</v>
+      </c>
+      <c r="P5" s="2">
+        <v>34750.400000000001</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>46911</v>
+      </c>
+      <c r="R5" s="2">
+        <v>48069</v>
+      </c>
+      <c r="S5" s="2">
+        <v>52610</v>
+      </c>
+      <c r="T5" s="2">
+        <v>53063</v>
+      </c>
+      <c r="U5" s="2">
+        <v>66252</v>
+      </c>
+      <c r="V5" s="2">
+        <v>80102</v>
+      </c>
+      <c r="W5" s="2">
+        <v>110497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B6" s="2">
+        <v>55.2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>73.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="E6" s="2">
+        <v>92.3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>146.1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2">
+        <v>127.2</v>
+      </c>
+      <c r="I6" s="12">
+        <f>annual_psy!I6</f>
+        <v>327.9</v>
+      </c>
+      <c r="J6" s="2">
+        <f>K6/1.72</f>
+        <v>294.18604651162792</v>
+      </c>
+      <c r="K6" s="2">
+        <v>506</v>
+      </c>
+      <c r="L6" s="2">
+        <v>669.1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>743.4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>898.1</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1136.0999999999999</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1840.8</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1894.7</v>
+      </c>
+      <c r="R6" s="11">
+        <v>2601</v>
+      </c>
+      <c r="S6" s="11">
+        <v>6996</v>
+      </c>
+      <c r="T6" s="11">
+        <v>4881</v>
+      </c>
+      <c r="U6" s="11">
+        <v>10876</v>
+      </c>
+      <c r="V6" s="11">
+        <v>15823</v>
+      </c>
+      <c r="W6" s="11">
+        <v>16939</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>468</v>
+      </c>
+      <c r="B7" s="2">
+        <f>B2-B5</f>
+        <v>-245.89999999999986</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:W7" si="0">C2-C5</f>
+        <v>-376.69999999999982</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>-268.19999999999982</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>-444.80000000000018</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>-816</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>-997.70000000000027</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>-183.80000000000018</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" ref="I7" si="1">I2-I5</f>
+        <v>-665.61320868043822</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>2120</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="0"/>
+        <v>2568</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>-726.39999999999782</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:O7" si="2">M2-M5</f>
+        <v>-2021.2000000000007</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="2"/>
+        <v>-1834</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="2"/>
+        <v>-1559.2000000000007</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" ref="P7:Q7" si="3">P2-P5</f>
+        <v>508.29999999999563</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="3"/>
+        <v>-1094.8000000000029</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" ref="R7:W7" si="4">R2-R5</f>
+        <v>-12136</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="4"/>
+        <v>-14405</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="4"/>
+        <v>-6422</v>
+      </c>
+      <c r="U7" s="2">
+        <f t="shared" si="4"/>
+        <v>-8325</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" si="4"/>
+        <v>-11141</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" si="4"/>
+        <v>-31252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B7+B6</f>
+        <v>-190.69999999999987</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:W8" si="5">C7+C6</f>
+        <v>-303.19999999999982</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="5"/>
+        <v>-191.59999999999982</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="5"/>
+        <v>-352.50000000000017</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="5"/>
+        <v>-669.9</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="5"/>
+        <v>-914.70000000000027</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="5"/>
+        <v>-56.600000000000179</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="5"/>
+        <v>-337.71320868043824</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="5"/>
+        <v>2414.1860465116279</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="5"/>
+        <v>3074</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="5"/>
+        <v>-57.299999999997794</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="5"/>
+        <v>-1277.8000000000006</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="5"/>
+        <v>-935.9</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="5"/>
+        <v>-423.10000000000082</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="5"/>
+        <v>2349.0999999999958</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="5"/>
+        <v>799.89999999999714</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="5"/>
+        <v>-9535</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="5"/>
+        <v>-7409</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" ref="T8" si="6">T7+T6</f>
+        <v>-1541</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" ref="U8" si="7">U7+U6</f>
+        <v>2551</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" ref="V8" si="8">V7+V6</f>
+        <v>4682</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" ref="W8" si="9">W7+W6</f>
+        <v>-14313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>

</xml_diff>